<commit_message>
01.08.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/August/Others/Cash.xlsx
+++ b/August/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 30.07.19</t>
+    <t>Date: 01.08.19</t>
   </si>
 </sst>
 </file>
@@ -467,47 +467,83 @@
     <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -515,13 +551,7 @@
     <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -536,21 +566,27 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -571,42 +607,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2054,7 +2054,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2076,60 +2076,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2138,10 +2138,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2156,10 +2156,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="36">
         <v>50</v>
       </c>
-      <c r="F6" s="32"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2175,10 +2175,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="36">
         <v>16</v>
       </c>
-      <c r="F7" s="32"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2194,10 +2194,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="36">
         <v>151</v>
       </c>
-      <c r="F8" s="32"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2213,10 +2213,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="36">
         <v>58</v>
       </c>
-      <c r="F9" s="32"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2232,8 +2232,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2249,8 +2249,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2263,10 +2263,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2313,58 +2313,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="34"/>
-      <c r="B19" s="34"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="35" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2374,11 +2374,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="36" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2453,60 +2453,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="29"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="30" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="30"/>
-      <c r="J28" s="30"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2515,10 +2515,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2533,10 +2533,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="32">
+      <c r="E32" s="36">
         <v>50</v>
       </c>
-      <c r="F32" s="32"/>
+      <c r="F32" s="36"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2552,10 +2552,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="32">
+      <c r="E33" s="36">
         <v>116</v>
       </c>
-      <c r="F33" s="32"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2571,10 +2571,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="32">
+      <c r="E34" s="36">
         <v>151</v>
       </c>
-      <c r="F34" s="32"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2590,10 +2590,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="32">
+      <c r="E35" s="36">
         <v>58</v>
       </c>
-      <c r="F35" s="32"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2609,8 +2609,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2626,8 +2626,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2640,10 +2640,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="39" t="s">
+      <c r="D38" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="40"/>
+      <c r="E38" s="33"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2690,58 +2690,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="41"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="41" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="41"/>
-      <c r="J42" s="41"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="34"/>
-      <c r="B43" s="34"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="34"/>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="34"/>
-      <c r="B44" s="34"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="34"/>
-      <c r="I44" s="34"/>
-      <c r="J44" s="34"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="34"/>
-      <c r="B45" s="34"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="34" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2751,11 +2751,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="36" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="37"/>
-      <c r="J46" s="37"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2783,14 +2783,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2803,24 +2813,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2833,7 +2833,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M40" sqref="M40"/>
+      <selection activeCell="H46" sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2851,77 +2851,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="66" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="66"/>
-      <c r="C1" s="66"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="66"/>
-      <c r="J1" s="66"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="68"/>
-      <c r="C4" s="68"/>
-      <c r="D4" s="68"/>
-      <c r="E4" s="68"/>
-      <c r="F4" s="68"/>
-      <c r="G4" s="68"/>
-      <c r="H4" s="68"/>
-      <c r="I4" s="68"/>
-      <c r="J4" s="68"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
       <c r="A5" s="26"/>
       <c r="B5" s="26"/>
       <c r="C5" s="26"/>
-      <c r="D5" s="72" t="s">
+      <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="73" t="s">
+      <c r="E5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="73"/>
-      <c r="G5" s="72" t="s">
+      <c r="F5" s="48"/>
+      <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
       <c r="H5" s="26"/>
@@ -2936,12 +2936,12 @@
         <v>1000</v>
       </c>
       <c r="E6" s="44">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="F6" s="44"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>94000</v>
+        <v>64000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2955,12 +2955,12 @@
         <v>500</v>
       </c>
       <c r="E7" s="44">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="F7" s="44"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>75000</v>
+        <v>100000</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2974,12 +2974,12 @@
         <v>100</v>
       </c>
       <c r="E8" s="44">
-        <v>300</v>
+        <v>140</v>
       </c>
       <c r="F8" s="44"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>30000</v>
+        <v>14000</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2992,13 +2992,11 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="44">
-        <v>120</v>
-      </c>
+      <c r="E9" s="44"/>
       <c r="F9" s="44"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3011,9 +3009,7 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="44">
-        <v>0</v>
-      </c>
+      <c r="E10" s="44"/>
       <c r="F10" s="44"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
@@ -3030,13 +3026,11 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="44">
-        <v>200</v>
-      </c>
+      <c r="E11" s="44"/>
       <c r="F11" s="44"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3046,14 +3040,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="45" t="s">
+      <c r="D12" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="45"/>
+      <c r="E12" s="51"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>207000</v>
+        <v>178000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3096,58 +3090,58 @@
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="69" t="s">
+      <c r="A16" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="69"/>
-      <c r="C16" s="71"/>
-      <c r="D16" s="71"/>
-      <c r="E16" s="71"/>
-      <c r="F16" s="71"/>
-      <c r="G16" s="71"/>
-      <c r="H16" s="69" t="s">
+      <c r="B16" s="49"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="69"/>
-      <c r="J16" s="69"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="69"/>
-      <c r="B17" s="69"/>
-      <c r="C17" s="71"/>
-      <c r="D17" s="71"/>
-      <c r="E17" s="71"/>
-      <c r="F17" s="71"/>
-      <c r="G17" s="71"/>
-      <c r="H17" s="69"/>
-      <c r="I17" s="69"/>
-      <c r="J17" s="69"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="69"/>
-      <c r="B18" s="69"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="71"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="71"/>
-      <c r="H18" s="69"/>
-      <c r="I18" s="69"/>
-      <c r="J18" s="69"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="69"/>
-      <c r="B19" s="69"/>
-      <c r="C19" s="71"/>
-      <c r="D19" s="71"/>
-      <c r="E19" s="71"/>
-      <c r="F19" s="71"/>
-      <c r="G19" s="71"/>
-      <c r="H19" s="74" t="s">
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="74"/>
-      <c r="J19" s="74"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="26"/>
@@ -3157,9 +3151,9 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="70"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="26"/>
@@ -3246,73 +3240,73 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="66" t="s">
+      <c r="A28" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="66"/>
-      <c r="C28" s="66"/>
-      <c r="D28" s="66"/>
-      <c r="E28" s="66"/>
-      <c r="F28" s="66"/>
-      <c r="G28" s="66"/>
-      <c r="H28" s="66"/>
-      <c r="I28" s="66"/>
-      <c r="J28" s="66"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="67" t="s">
+      <c r="A29" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="67"/>
-      <c r="C29" s="67"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="67"/>
-      <c r="F29" s="67"/>
-      <c r="G29" s="67"/>
-      <c r="H29" s="67"/>
-      <c r="I29" s="67"/>
-      <c r="J29" s="67"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="68" t="s">
+      <c r="A30" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="68"/>
-      <c r="C30" s="68"/>
-      <c r="D30" s="68"/>
-      <c r="E30" s="68"/>
-      <c r="F30" s="68"/>
-      <c r="G30" s="68"/>
-      <c r="H30" s="68"/>
-      <c r="I30" s="68"/>
-      <c r="J30" s="68"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="68" t="s">
+      <c r="A31" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="68"/>
-      <c r="C31" s="68"/>
-      <c r="D31" s="68"/>
-      <c r="E31" s="68"/>
-      <c r="F31" s="68"/>
-      <c r="G31" s="68"/>
-      <c r="H31" s="68"/>
-      <c r="I31" s="68"/>
-      <c r="J31" s="68"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
       <c r="B32" s="26"/>
       <c r="C32" s="26"/>
-      <c r="D32" s="72" t="s">
+      <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="73" t="s">
+      <c r="E32" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="73"/>
-      <c r="G32" s="72" t="s">
+      <c r="F32" s="48"/>
+      <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
       <c r="H32" s="26"/>
@@ -3327,12 +3321,12 @@
         <v>1000</v>
       </c>
       <c r="E33" s="44">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="F33" s="44"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>94000</v>
+        <v>64000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3346,12 +3340,12 @@
         <v>500</v>
       </c>
       <c r="E34" s="44">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="F34" s="44"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>75000</v>
+        <v>100000</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3365,12 +3359,12 @@
         <v>100</v>
       </c>
       <c r="E35" s="44">
-        <v>300</v>
+        <v>140</v>
       </c>
       <c r="F35" s="44"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>30000</v>
+        <v>14000</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3383,13 +3377,11 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="44">
-        <v>120</v>
-      </c>
+      <c r="E36" s="44"/>
       <c r="F36" s="44"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>6000</v>
+        <v>0</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3402,9 +3394,7 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="44">
-        <v>0</v>
-      </c>
+      <c r="E37" s="44"/>
       <c r="F37" s="44"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
@@ -3421,13 +3411,11 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="44">
-        <v>200</v>
-      </c>
+      <c r="E38" s="44"/>
       <c r="F38" s="44"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3437,14 +3425,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="42" t="s">
+      <c r="D39" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="43"/>
+      <c r="E39" s="55"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>207000</v>
+        <v>178000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3487,58 +3475,58 @@
       <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="69" t="s">
+      <c r="A43" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="69"/>
-      <c r="C43" s="71"/>
-      <c r="D43" s="71"/>
-      <c r="E43" s="71"/>
-      <c r="F43" s="71"/>
-      <c r="G43" s="71"/>
-      <c r="H43" s="69" t="s">
+      <c r="B43" s="49"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="28"/>
+      <c r="H43" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="69"/>
-      <c r="J43" s="69"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="46"/>
-      <c r="B44" s="46"/>
+      <c r="A44" s="53"/>
+      <c r="B44" s="53"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="46"/>
-      <c r="I44" s="46"/>
-      <c r="J44" s="46"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="53"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="46"/>
-      <c r="B45" s="46"/>
+      <c r="A45" s="53"/>
+      <c r="B45" s="53"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="46"/>
-      <c r="I45" s="46"/>
-      <c r="J45" s="46"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="53"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
-      <c r="A46" s="69"/>
-      <c r="B46" s="69"/>
-      <c r="C46" s="71"/>
-      <c r="D46" s="71"/>
-      <c r="E46" s="71"/>
-      <c r="F46" s="71"/>
-      <c r="G46" s="71"/>
-      <c r="H46" s="74" t="s">
+      <c r="A46" s="49"/>
+      <c r="B46" s="49"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="28"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="28"/>
+      <c r="G46" s="28"/>
+      <c r="H46" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="74"/>
-      <c r="J46" s="74"/>
+      <c r="I46" s="50"/>
+      <c r="J46" s="50"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3548,9 +3536,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="36"/>
-      <c r="I47" s="37"/>
-      <c r="J47" s="37"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3578,28 +3566,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3616,6 +3582,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3646,63 +3634,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3712,10 +3700,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3730,10 +3718,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="36">
         <v>68</v>
       </c>
-      <c r="F6" s="32"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3749,10 +3737,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="36">
         <v>135</v>
       </c>
-      <c r="F7" s="32"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3768,10 +3756,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="36">
         <v>53</v>
       </c>
-      <c r="F8" s="32"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3787,10 +3775,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="36">
         <v>2</v>
       </c>
-      <c r="F9" s="32"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3806,10 +3794,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="36">
         <v>5</v>
       </c>
-      <c r="F10" s="32"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3825,8 +3813,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3839,10 +3827,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3889,76 +3877,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="34"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="35" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="47"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="36" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4033,60 +4021,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="29"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="30" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="30"/>
-      <c r="J28" s="30"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4095,10 +4083,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="51" t="s">
+      <c r="E31" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="51"/>
+      <c r="F31" s="56"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4113,10 +4101,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="50">
+      <c r="E32" s="60">
         <v>68</v>
       </c>
-      <c r="F32" s="50"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4132,10 +4120,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="50">
+      <c r="E33" s="60">
         <v>135</v>
       </c>
-      <c r="F33" s="50"/>
+      <c r="F33" s="60"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4151,10 +4139,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="50">
+      <c r="E34" s="60">
         <v>53</v>
       </c>
-      <c r="F34" s="50"/>
+      <c r="F34" s="60"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4170,10 +4158,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="50">
+      <c r="E35" s="60">
         <v>2</v>
       </c>
-      <c r="F35" s="50"/>
+      <c r="F35" s="60"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4189,10 +4177,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="50">
+      <c r="E36" s="60">
         <v>5</v>
       </c>
-      <c r="F36" s="50"/>
+      <c r="F36" s="60"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4208,8 +4196,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="50"/>
-      <c r="F37" s="50"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4222,10 +4210,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="49" t="s">
+      <c r="D38" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="49"/>
+      <c r="E38" s="59"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4272,76 +4260,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="41"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="41" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="41"/>
-      <c r="J42" s="41"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="34"/>
-      <c r="B43" s="34"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="34"/>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="34"/>
-      <c r="B44" s="34"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="34"/>
-      <c r="I44" s="34"/>
-      <c r="J44" s="34"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="34" t="s">
+      <c r="A45" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="34"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="34" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="48" t="s">
+      <c r="A46" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="48"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="36" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="37"/>
-      <c r="J46" s="37"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4369,30 +4357,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4409,6 +4373,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4440,63 +4428,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4506,10 +4494,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="28"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4524,10 +4512,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="36">
         <v>44</v>
       </c>
-      <c r="F6" s="32"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4543,10 +4531,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="36">
         <v>118</v>
       </c>
-      <c r="F7" s="32"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4562,10 +4550,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="36">
         <v>510</v>
       </c>
-      <c r="F8" s="32"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4581,8 +4569,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4598,8 +4586,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4615,8 +4603,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4629,10 +4617,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="28"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4679,72 +4667,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="33" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="34"/>
-      <c r="B19" s="34"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="35" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="53"/>
-      <c r="B20" s="53"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="61"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="36" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4819,60 +4807,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="29"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="30" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="30"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="30"/>
-      <c r="J28" s="30"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4881,10 +4869,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="28" t="s">
+      <c r="E31" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4899,10 +4887,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="32">
+      <c r="E32" s="36">
         <v>44</v>
       </c>
-      <c r="F32" s="32"/>
+      <c r="F32" s="36"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4918,10 +4906,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="32">
+      <c r="E33" s="36">
         <v>118</v>
       </c>
-      <c r="F33" s="32"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4937,10 +4925,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="32">
+      <c r="E34" s="36">
         <v>510</v>
       </c>
-      <c r="F34" s="32"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4956,8 +4944,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="32"/>
-      <c r="F35" s="32"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4973,8 +4961,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4990,8 +4978,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5004,10 +4992,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="52" t="s">
+      <c r="D38" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="52"/>
+      <c r="E38" s="62"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5054,72 +5042,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="41" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="41"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="41" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="41"/>
-      <c r="J42" s="41"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="34"/>
-      <c r="B43" s="34"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="34"/>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="34"/>
-      <c r="B44" s="34"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="34"/>
-      <c r="I44" s="34"/>
-      <c r="J44" s="34"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="34"/>
-      <c r="B45" s="34"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="34" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="48"/>
-      <c r="B46" s="48"/>
+      <c r="A46" s="58"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="36" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="37"/>
-      <c r="J46" s="37"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5147,6 +5135,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5159,34 +5175,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5211,64 +5199,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="31"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5279,8 +5267,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="32"/>
-      <c r="F6" s="32"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5291,8 +5279,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5303,8 +5291,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="32"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5315,8 +5303,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5327,8 +5315,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5339,8 +5327,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="32"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5350,8 +5338,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5395,52 +5383,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="33"/>
-      <c r="B16" s="33"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="33"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="33"/>
-      <c r="I17" s="33"/>
-      <c r="J17" s="33"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="33"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="34"/>
-      <c r="B19" s="34"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5450,9 +5438,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5539,60 +5527,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="30"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="30"/>
-      <c r="J29" s="30"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5603,10 +5591,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="51" t="s">
+      <c r="E32" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="51"/>
+      <c r="F32" s="56"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5621,10 +5609,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="32">
+      <c r="E33" s="36">
         <v>30</v>
       </c>
-      <c r="F33" s="32"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5640,10 +5628,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="32">
+      <c r="E34" s="36">
         <v>35</v>
       </c>
-      <c r="F34" s="32"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5659,10 +5647,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="32">
+      <c r="E35" s="36">
         <v>425</v>
       </c>
-      <c r="F35" s="32"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5678,8 +5666,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="32"/>
-      <c r="F36" s="32"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5695,8 +5683,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="50"/>
-      <c r="F37" s="50"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5712,10 +5700,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="50">
+      <c r="E38" s="60">
         <v>100</v>
       </c>
-      <c r="F38" s="50"/>
+      <c r="F38" s="60"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5728,10 +5716,10 @@
       <c r="A39" s="6"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="54" t="s">
+      <c r="D39" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="55"/>
+      <c r="E39" s="64"/>
       <c r="F39" s="20"/>
       <c r="G39" s="20">
         <f>SUM(G33:G38)</f>
@@ -5778,58 +5766,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="41" t="s">
+      <c r="A43" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="41"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="41" t="s">
+      <c r="H43" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="34"/>
-      <c r="B44" s="34"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="34"/>
-      <c r="I44" s="34"/>
-      <c r="J44" s="34"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="34"/>
-      <c r="B45" s="34"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="34"/>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="34"/>
-      <c r="B46" s="34"/>
+      <c r="A46" s="35"/>
+      <c r="B46" s="35"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="34" t="s">
+      <c r="H46" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="41"/>
-      <c r="J46" s="41"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5839,20 +5827,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="36"/>
-      <c r="I47" s="37"/>
-      <c r="J47" s="37"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -5865,24 +5863,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5908,128 +5896,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="64">
+      <c r="A5" s="67">
         <v>1</v>
       </c>
-      <c r="B5" s="56" t="s">
+      <c r="B5" s="68" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="56"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="63">
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="66">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="64"/>
-      <c r="B6" s="56"/>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="63"/>
+      <c r="A6" s="67"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="66"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="64">
+      <c r="A7" s="67">
         <v>2</v>
       </c>
-      <c r="B7" s="56" t="s">
+      <c r="B7" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="56"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="56"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="63">
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="66">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="64"/>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="56"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="56"/>
-      <c r="G8" s="63"/>
+      <c r="A8" s="67"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="66"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="64">
+      <c r="A9" s="67">
         <v>3</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="68" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="63">
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="66">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="64"/>
-      <c r="B10" s="56"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="63"/>
+      <c r="A10" s="67"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="66"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="64">
+      <c r="A11" s="67">
         <v>4</v>
       </c>
-      <c r="B11" s="57" t="s">
+      <c r="B11" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="63">
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
+      <c r="E11" s="70"/>
+      <c r="F11" s="71"/>
+      <c r="G11" s="66">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="64"/>
-      <c r="B12" s="60"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="62"/>
-      <c r="G12" s="63"/>
+      <c r="A12" s="67"/>
+      <c r="B12" s="72"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="74"/>
+      <c r="G12" s="66"/>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="65" t="s">
@@ -6040,7 +6028,7 @@
       <c r="D13" s="65"/>
       <c r="E13" s="65"/>
       <c r="F13" s="65"/>
-      <c r="G13" s="63">
+      <c r="G13" s="66">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
@@ -6052,33 +6040,33 @@
       <c r="D14" s="65"/>
       <c r="E14" s="65"/>
       <c r="F14" s="65"/>
-      <c r="G14" s="63"/>
+      <c r="G14" s="66"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="38" t="s">
+      <c r="A23" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="38"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="38"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="31"/>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6089,10 +6077,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="51" t="s">
+      <c r="E25" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="51"/>
+      <c r="F25" s="56"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6107,8 +6095,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6124,10 +6112,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="32">
+      <c r="E27" s="36">
         <v>30</v>
       </c>
-      <c r="F27" s="32"/>
+      <c r="F27" s="36"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6143,8 +6131,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6160,10 +6148,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="32">
+      <c r="E29" s="36">
         <v>5</v>
       </c>
-      <c r="F29" s="32"/>
+      <c r="F29" s="36"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6179,8 +6167,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="50"/>
-      <c r="F30" s="50"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6196,10 +6184,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="50">
+      <c r="E31" s="60">
         <v>2</v>
       </c>
-      <c r="F31" s="50"/>
+      <c r="F31" s="60"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6212,10 +6200,10 @@
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="54" t="s">
+      <c r="D32" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="55"/>
+      <c r="E32" s="64"/>
       <c r="F32" s="20"/>
       <c r="G32" s="20">
         <f>SUM(G26:G31)</f>
@@ -6262,58 +6250,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="41" t="s">
+      <c r="A36" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="41"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="41" t="s">
+      <c r="H36" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="41"/>
-      <c r="J36" s="41"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="34"/>
-      <c r="B37" s="34"/>
+      <c r="A37" s="35"/>
+      <c r="B37" s="35"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="34"/>
-      <c r="I37" s="34"/>
-      <c r="J37" s="34"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="34"/>
-      <c r="B38" s="34"/>
+      <c r="A38" s="35"/>
+      <c r="B38" s="35"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="34"/>
-      <c r="I38" s="34"/>
-      <c r="J38" s="34"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="35"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="34"/>
-      <c r="B39" s="34"/>
+      <c r="A39" s="35"/>
+      <c r="B39" s="35"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="34" t="s">
+      <c r="H39" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="41"/>
-      <c r="J39" s="41"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6323,33 +6311,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="37"/>
-      <c r="J40" s="37"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6362,6 +6329,27 @@
     <mergeCell ref="A7:A8"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
04.08.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/August/Others/Cash.xlsx
+++ b/August/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 01.08.19</t>
+    <t>Date: 03.08.19</t>
   </si>
 </sst>
 </file>
@@ -473,12 +473,39 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -488,125 +515,98 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2054,7 +2054,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2076,60 +2076,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2138,10 +2138,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2156,10 +2156,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>50</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2175,10 +2175,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>16</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2194,10 +2194,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>151</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2213,10 +2213,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="34">
         <v>58</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2232,8 +2232,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2249,8 +2249,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2263,10 +2263,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2313,58 +2313,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2374,11 +2374,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2453,60 +2453,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2515,10 +2515,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="41"/>
+      <c r="F31" s="30"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2533,10 +2533,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="34">
         <v>50</v>
       </c>
-      <c r="F32" s="36"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2552,10 +2552,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>116</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2571,10 +2571,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>151</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2590,10 +2590,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="34">
         <v>58</v>
       </c>
-      <c r="F35" s="36"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2609,8 +2609,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2626,8 +2626,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2640,10 +2640,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="32" t="s">
+      <c r="D38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="33"/>
+      <c r="E38" s="42"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2690,58 +2690,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2751,11 +2751,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2783,6 +2783,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2795,32 +2821,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2832,8 +2832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H46" sqref="A1:J46"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2851,63 +2851,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2917,10 +2917,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="48"/>
+      <c r="F5" s="53"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2935,13 +2935,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="44">
-        <v>64</v>
-      </c>
-      <c r="F6" s="44"/>
+      <c r="E6" s="54">
+        <v>79</v>
+      </c>
+      <c r="F6" s="54"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>64000</v>
+        <v>79000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2954,13 +2954,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="44">
-        <v>200</v>
-      </c>
-      <c r="F7" s="44"/>
+      <c r="E7" s="54">
+        <v>187</v>
+      </c>
+      <c r="F7" s="54"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>100000</v>
+        <v>93500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2973,13 +2973,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="44">
-        <v>140</v>
-      </c>
-      <c r="F8" s="44"/>
+      <c r="E8" s="54">
+        <v>237</v>
+      </c>
+      <c r="F8" s="54"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>14000</v>
+        <v>23700</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2992,11 +2992,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
+      <c r="E9" s="54">
+        <v>116</v>
+      </c>
+      <c r="F9" s="54"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5800</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3009,8 +3011,8 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3026,8 +3028,8 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3040,14 +3042,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="51"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>178000</v>
+        <v>202000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3090,58 +3092,58 @@
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="49"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="49" t="s">
+      <c r="H16" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="46"/>
+      <c r="B17" s="46"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="49"/>
-      <c r="B19" s="49"/>
+      <c r="A19" s="46"/>
+      <c r="B19" s="46"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="50" t="s">
+      <c r="H19" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="26"/>
@@ -3151,9 +3153,9 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="26"/>
@@ -3240,60 +3242,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="51"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="52"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="47" t="s">
+      <c r="A31" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="47"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3302,10 +3304,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="48" t="s">
+      <c r="E32" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="48"/>
+      <c r="F32" s="53"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3320,13 +3322,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="44">
-        <v>64</v>
-      </c>
-      <c r="F33" s="44"/>
+      <c r="E33" s="54">
+        <v>79</v>
+      </c>
+      <c r="F33" s="54"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>64000</v>
+        <v>79000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3339,13 +3341,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="44">
-        <v>200</v>
-      </c>
-      <c r="F34" s="44"/>
+      <c r="E34" s="54">
+        <v>187</v>
+      </c>
+      <c r="F34" s="54"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>100000</v>
+        <v>93500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3358,13 +3360,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="44">
-        <v>140</v>
-      </c>
-      <c r="F35" s="44"/>
+      <c r="E35" s="54">
+        <v>237</v>
+      </c>
+      <c r="F35" s="54"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>14000</v>
+        <v>23700</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3377,11 +3379,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="44"/>
-      <c r="F36" s="44"/>
+      <c r="E36" s="54">
+        <v>116</v>
+      </c>
+      <c r="F36" s="54"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5800</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3394,8 +3398,8 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="54"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -3411,8 +3415,8 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="44"/>
-      <c r="F38" s="44"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="54"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3425,14 +3429,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="54" t="s">
+      <c r="D39" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="55"/>
+      <c r="E39" s="49"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>178000</v>
+        <v>202000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3475,58 +3479,58 @@
       <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="49" t="s">
+      <c r="A43" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="49"/>
+      <c r="B43" s="46"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="49" t="s">
+      <c r="H43" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="49"/>
-      <c r="J43" s="49"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="46"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="53"/>
-      <c r="B44" s="53"/>
+      <c r="A44" s="45"/>
+      <c r="B44" s="45"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="53"/>
-      <c r="I44" s="53"/>
-      <c r="J44" s="53"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
+      <c r="J44" s="45"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="53"/>
-      <c r="B45" s="53"/>
+      <c r="A45" s="45"/>
+      <c r="B45" s="45"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="53"/>
-      <c r="I45" s="53"/>
-      <c r="J45" s="53"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="45"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
-      <c r="A46" s="49"/>
-      <c r="B46" s="49"/>
+      <c r="A46" s="46"/>
+      <c r="B46" s="46"/>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="50" t="s">
+      <c r="H46" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="50"/>
-      <c r="J46" s="50"/>
+      <c r="I46" s="47"/>
+      <c r="J46" s="47"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3536,9 +3540,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3566,6 +3570,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3582,28 +3608,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3634,63 +3638,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3700,10 +3704,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3718,10 +3722,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>68</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3737,10 +3741,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>135</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3756,10 +3760,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>53</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3775,10 +3779,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="34">
         <v>2</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3794,10 +3798,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="36">
+      <c r="E10" s="34">
         <v>5</v>
       </c>
-      <c r="F10" s="36"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3813,8 +3817,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3827,10 +3831,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3877,76 +3881,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="35"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="57"/>
+      <c r="B20" s="56"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4021,60 +4025,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4083,10 +4087,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="56" t="s">
+      <c r="E31" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="56"/>
+      <c r="F31" s="60"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4101,10 +4105,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="60">
+      <c r="E32" s="59">
         <v>68</v>
       </c>
-      <c r="F32" s="60"/>
+      <c r="F32" s="59"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4120,10 +4124,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="60">
+      <c r="E33" s="59">
         <v>135</v>
       </c>
-      <c r="F33" s="60"/>
+      <c r="F33" s="59"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4139,10 +4143,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="60">
+      <c r="E34" s="59">
         <v>53</v>
       </c>
-      <c r="F34" s="60"/>
+      <c r="F34" s="59"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4158,10 +4162,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="60">
+      <c r="E35" s="59">
         <v>2</v>
       </c>
-      <c r="F35" s="60"/>
+      <c r="F35" s="59"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4177,10 +4181,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="60">
+      <c r="E36" s="59">
         <v>5</v>
       </c>
-      <c r="F36" s="60"/>
+      <c r="F36" s="59"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4196,8 +4200,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4210,10 +4214,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="59" t="s">
+      <c r="D38" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="59"/>
+      <c r="E38" s="58"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4260,76 +4264,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="35"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58" t="s">
+      <c r="A46" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="58"/>
+      <c r="B46" s="57"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4357,6 +4361,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4373,30 +4401,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4428,63 +4432,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4494,10 +4498,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4512,10 +4516,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>44</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4531,10 +4535,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>118</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4550,10 +4554,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>510</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4569,8 +4573,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4586,8 +4590,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4603,8 +4607,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4617,10 +4621,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4667,72 +4671,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="61"/>
-      <c r="B20" s="61"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="62"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4807,60 +4811,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4869,10 +4873,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="41"/>
+      <c r="F31" s="30"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4887,10 +4891,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="34">
         <v>44</v>
       </c>
-      <c r="F32" s="36"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4906,10 +4910,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>118</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4925,10 +4929,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>510</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4944,8 +4948,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4961,8 +4965,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4978,8 +4982,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4992,10 +4996,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="62" t="s">
+      <c r="D38" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="62"/>
+      <c r="E38" s="61"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5042,72 +5046,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58"/>
-      <c r="B46" s="58"/>
+      <c r="A46" s="57"/>
+      <c r="B46" s="57"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5135,16 +5139,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5157,24 +5169,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5199,64 +5203,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5267,8 +5271,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5279,8 +5283,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5291,8 +5295,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5303,8 +5307,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5315,8 +5319,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5327,8 +5331,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5338,8 +5342,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5383,52 +5387,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42"/>
-      <c r="B16" s="42"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5438,9 +5442,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5527,60 +5531,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5591,10 +5595,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="56" t="s">
+      <c r="E32" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="56"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5609,10 +5613,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>30</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5628,10 +5632,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>35</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5647,10 +5651,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="34">
         <v>425</v>
       </c>
-      <c r="F35" s="36"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5666,8 +5670,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5683,8 +5687,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5700,10 +5704,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="60">
+      <c r="E38" s="59">
         <v>100</v>
       </c>
-      <c r="F38" s="60"/>
+      <c r="F38" s="59"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5766,58 +5770,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="34"/>
+      <c r="B43" s="43"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="34" t="s">
+      <c r="H43" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="35"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="36"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="35"/>
-      <c r="B46" s="35"/>
+      <c r="A46" s="36"/>
+      <c r="B46" s="36"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
+      <c r="I46" s="43"/>
+      <c r="J46" s="43"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5827,12 +5831,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5845,32 +5875,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5896,177 +5900,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="67">
+      <c r="A5" s="73">
         <v>1</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="66">
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="72">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="67"/>
-      <c r="B6" s="68"/>
-      <c r="C6" s="68"/>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="66"/>
+      <c r="A6" s="73"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="72"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="67">
+      <c r="A7" s="73">
         <v>2</v>
       </c>
-      <c r="B7" s="68" t="s">
+      <c r="B7" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="68"/>
-      <c r="D7" s="68"/>
-      <c r="E7" s="68"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="66">
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="72">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="67"/>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="66"/>
+      <c r="A8" s="73"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="72"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="67">
+      <c r="A9" s="73">
         <v>3</v>
       </c>
-      <c r="B9" s="68" t="s">
+      <c r="B9" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="68"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="68"/>
-      <c r="G9" s="66">
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="72">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="67"/>
-      <c r="B10" s="68"/>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="66"/>
+      <c r="A10" s="73"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="72"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="67">
+      <c r="A11" s="73">
         <v>4</v>
       </c>
-      <c r="B11" s="69" t="s">
+      <c r="B11" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="70"/>
-      <c r="D11" s="70"/>
-      <c r="E11" s="70"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="66">
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="72">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="67"/>
-      <c r="B12" s="72"/>
-      <c r="C12" s="73"/>
-      <c r="D12" s="73"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="66"/>
+      <c r="A12" s="73"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="72"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="65" t="s">
+      <c r="A13" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="65"/>
-      <c r="C13" s="65"/>
-      <c r="D13" s="65"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="66">
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="72">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="65"/>
-      <c r="B14" s="65"/>
-      <c r="C14" s="65"/>
-      <c r="D14" s="65"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="65"/>
-      <c r="G14" s="66"/>
+      <c r="A14" s="74"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="72"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="40"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6077,10 +6081,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="56" t="s">
+      <c r="E25" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="56"/>
+      <c r="F25" s="60"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6095,8 +6099,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6112,10 +6116,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="36">
+      <c r="E27" s="34">
         <v>30</v>
       </c>
-      <c r="F27" s="36"/>
+      <c r="F27" s="34"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6131,8 +6135,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6148,10 +6152,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="36">
+      <c r="E29" s="34">
         <v>5</v>
       </c>
-      <c r="F29" s="36"/>
+      <c r="F29" s="34"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6167,8 +6171,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="59"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6184,10 +6188,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="60">
+      <c r="E31" s="59">
         <v>2</v>
       </c>
-      <c r="F31" s="60"/>
+      <c r="F31" s="59"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6250,58 +6254,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="34"/>
+      <c r="B36" s="43"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="34" t="s">
+      <c r="H36" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="35"/>
-      <c r="B37" s="35"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="36"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="35"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="36"/>
+      <c r="J37" s="36"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="35"/>
-      <c r="B38" s="35"/>
+      <c r="A38" s="36"/>
+      <c r="B38" s="36"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="35"/>
-      <c r="J38" s="35"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="36"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="35"/>
-      <c r="B39" s="35"/>
+      <c r="A39" s="36"/>
+      <c r="B39" s="36"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="35" t="s">
+      <c r="H39" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
+      <c r="I39" s="43"/>
+      <c r="J39" s="43"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6311,12 +6315,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="31"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6333,23 +6354,6 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
05.08.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/August/Others/Cash.xlsx
+++ b/August/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 03.08.19</t>
+    <t>Date: 05.08.19</t>
   </si>
 </sst>
 </file>
@@ -473,47 +473,71 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -521,34 +545,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -563,15 +566,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -579,6 +579,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -600,12 +606,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2054,7 +2054,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2076,60 +2076,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2138,10 +2138,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2156,10 +2156,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>50</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2175,10 +2175,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>16</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2194,10 +2194,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>151</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2213,10 +2213,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="36">
         <v>58</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2232,8 +2232,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2249,8 +2249,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2263,10 +2263,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2313,58 +2313,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2374,11 +2374,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2453,60 +2453,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2515,10 +2515,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="30"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2533,10 +2533,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="36">
         <v>50</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="36"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2552,10 +2552,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>116</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2571,10 +2571,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>151</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2590,10 +2590,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="36">
         <v>58</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2609,8 +2609,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2626,8 +2626,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2640,10 +2640,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="41" t="s">
+      <c r="D38" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="42"/>
+      <c r="E38" s="33"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2690,58 +2690,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2751,11 +2751,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2783,14 +2783,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2803,24 +2813,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2832,8 +2832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:J28"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="H46" sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2851,63 +2851,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2917,10 +2917,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="53"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2935,13 +2935,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="54">
-        <v>79</v>
-      </c>
-      <c r="F6" s="54"/>
+      <c r="E6" s="44">
+        <v>64</v>
+      </c>
+      <c r="F6" s="44"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>79000</v>
+        <v>64000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2954,13 +2954,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="54">
-        <v>187</v>
-      </c>
-      <c r="F7" s="54"/>
+      <c r="E7" s="44">
+        <v>108</v>
+      </c>
+      <c r="F7" s="44"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>93500</v>
+        <v>54000</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2973,13 +2973,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="54">
-        <v>237</v>
-      </c>
-      <c r="F8" s="54"/>
+      <c r="E8" s="44">
+        <v>180</v>
+      </c>
+      <c r="F8" s="44"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>23700</v>
+        <v>18000</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2992,13 +2992,11 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="54">
-        <v>116</v>
-      </c>
-      <c r="F9" s="54"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>5800</v>
+        <v>0</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3011,11 +3009,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
+      <c r="E10" s="44">
+        <v>200</v>
+      </c>
+      <c r="F10" s="44"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3028,8 +3028,8 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3042,14 +3042,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="55"/>
+      <c r="E12" s="51"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>202000</v>
+        <v>140000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3092,58 +3092,58 @@
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="46"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="46" t="s">
+      <c r="H16" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="46"/>
-      <c r="B17" s="46"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="46"/>
-      <c r="B18" s="46"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="46"/>
-      <c r="B19" s="46"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="47" t="s">
+      <c r="H19" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="26"/>
@@ -3153,9 +3153,9 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="26"/>
@@ -3242,60 +3242,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="50"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="50"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="51"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="52" t="s">
+      <c r="A30" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="52"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="52"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="52" t="s">
+      <c r="A31" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="52"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="52"/>
-      <c r="I31" s="52"/>
-      <c r="J31" s="52"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3304,10 +3304,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="53" t="s">
+      <c r="E32" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="53"/>
+      <c r="F32" s="48"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3322,13 +3322,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="54">
-        <v>79</v>
-      </c>
-      <c r="F33" s="54"/>
+      <c r="E33" s="44">
+        <v>64</v>
+      </c>
+      <c r="F33" s="44"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>79000</v>
+        <v>64000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3341,13 +3341,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="54">
-        <v>187</v>
-      </c>
-      <c r="F34" s="54"/>
+      <c r="E34" s="44">
+        <v>108</v>
+      </c>
+      <c r="F34" s="44"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>93500</v>
+        <v>54000</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3360,13 +3360,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="54">
-        <v>237</v>
-      </c>
-      <c r="F35" s="54"/>
+      <c r="E35" s="44">
+        <v>180</v>
+      </c>
+      <c r="F35" s="44"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>23700</v>
+        <v>18000</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3379,13 +3379,11 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="54">
-        <v>116</v>
-      </c>
-      <c r="F36" s="54"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="44"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>5800</v>
+        <v>0</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3398,11 +3396,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
+      <c r="E37" s="44">
+        <v>200</v>
+      </c>
+      <c r="F37" s="44"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>0</v>
+        <v>4000</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3415,8 +3415,8 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="54"/>
-      <c r="F38" s="54"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="44"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3429,14 +3429,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="48" t="s">
+      <c r="D39" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="49"/>
+      <c r="E39" s="55"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>202000</v>
+        <v>140000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3479,58 +3479,58 @@
       <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="46" t="s">
+      <c r="A43" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="46"/>
+      <c r="B43" s="49"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="46" t="s">
+      <c r="H43" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="46"/>
-      <c r="J43" s="46"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="45"/>
-      <c r="B44" s="45"/>
+      <c r="A44" s="53"/>
+      <c r="B44" s="53"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="45"/>
-      <c r="I44" s="45"/>
-      <c r="J44" s="45"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="53"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="45"/>
-      <c r="B45" s="45"/>
+      <c r="A45" s="53"/>
+      <c r="B45" s="53"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="45"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="53"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
-      <c r="A46" s="46"/>
-      <c r="B46" s="46"/>
+      <c r="A46" s="49"/>
+      <c r="B46" s="49"/>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="47" t="s">
+      <c r="H46" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="47"/>
-      <c r="J46" s="47"/>
+      <c r="I46" s="50"/>
+      <c r="J46" s="50"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3540,9 +3540,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3570,28 +3570,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3608,6 +3586,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3638,63 +3638,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3704,10 +3704,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3722,10 +3722,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>68</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3741,10 +3741,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>135</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3760,10 +3760,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>53</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3779,10 +3779,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="36">
         <v>2</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3798,10 +3798,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="36">
         <v>5</v>
       </c>
-      <c r="F10" s="34"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3817,8 +3817,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3831,10 +3831,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3881,76 +3881,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="36"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="56" t="s">
+      <c r="A20" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="56"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4025,60 +4025,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4087,10 +4087,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="60" t="s">
+      <c r="E31" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="60"/>
+      <c r="F31" s="56"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4105,10 +4105,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="59">
+      <c r="E32" s="60">
         <v>68</v>
       </c>
-      <c r="F32" s="59"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4124,10 +4124,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="59">
+      <c r="E33" s="60">
         <v>135</v>
       </c>
-      <c r="F33" s="59"/>
+      <c r="F33" s="60"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4143,10 +4143,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="59">
+      <c r="E34" s="60">
         <v>53</v>
       </c>
-      <c r="F34" s="59"/>
+      <c r="F34" s="60"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4162,10 +4162,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="59">
+      <c r="E35" s="60">
         <v>2</v>
       </c>
-      <c r="F35" s="59"/>
+      <c r="F35" s="60"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4181,10 +4181,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="59">
+      <c r="E36" s="60">
         <v>5</v>
       </c>
-      <c r="F36" s="59"/>
+      <c r="F36" s="60"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4200,8 +4200,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4214,10 +4214,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="58" t="s">
+      <c r="D38" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="58"/>
+      <c r="E38" s="59"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4264,76 +4264,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="36" t="s">
+      <c r="A45" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="36"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="57" t="s">
+      <c r="A46" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="57"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4361,30 +4361,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4401,6 +4377,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4432,63 +4432,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4498,10 +4498,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4516,10 +4516,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>44</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4535,10 +4535,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>118</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4554,10 +4554,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>510</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4573,8 +4573,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4590,8 +4590,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4607,8 +4607,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4621,10 +4621,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4671,72 +4671,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="62"/>
-      <c r="B20" s="62"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="61"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4811,60 +4811,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4873,10 +4873,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="30"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4891,10 +4891,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="36">
         <v>44</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="36"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4910,10 +4910,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>118</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4929,10 +4929,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>510</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4948,8 +4948,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4965,8 +4965,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4982,8 +4982,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4996,10 +4996,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="61" t="s">
+      <c r="D38" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="61"/>
+      <c r="E38" s="62"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5046,72 +5046,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="57"/>
-      <c r="B46" s="57"/>
+      <c r="A46" s="58"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5139,6 +5139,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5151,34 +5179,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5203,64 +5203,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5271,8 +5271,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5283,8 +5283,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5295,8 +5295,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5307,8 +5307,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5319,8 +5319,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5331,8 +5331,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5342,8 +5342,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5387,52 +5387,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5442,9 +5442,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5531,60 +5531,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5595,10 +5595,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="60" t="s">
+      <c r="E32" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="60"/>
+      <c r="F32" s="56"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5613,10 +5613,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>30</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5632,10 +5632,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>35</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5651,10 +5651,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="36">
         <v>425</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5670,8 +5670,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5687,8 +5687,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5704,10 +5704,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="59">
+      <c r="E38" s="60">
         <v>100</v>
       </c>
-      <c r="F38" s="59"/>
+      <c r="F38" s="60"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5770,58 +5770,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="43"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="43" t="s">
+      <c r="H43" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="36"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="36"/>
-      <c r="B46" s="36"/>
+      <c r="A46" s="35"/>
+      <c r="B46" s="35"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="36" t="s">
+      <c r="H46" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="43"/>
-      <c r="J46" s="43"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5831,20 +5831,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -5857,24 +5867,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5900,177 +5900,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="73">
+      <c r="A5" s="74">
         <v>1</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="72">
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="65">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="73"/>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="72"/>
+      <c r="A6" s="74"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="65"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="73">
+      <c r="A7" s="74">
         <v>2</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="72">
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="65">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="73"/>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="72"/>
+      <c r="A8" s="74"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="65"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="73">
+      <c r="A9" s="74">
         <v>3</v>
       </c>
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="72">
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="65">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="73"/>
-      <c r="B10" s="65"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="72"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="65"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="73">
+      <c r="A11" s="74">
         <v>4</v>
       </c>
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="72">
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="65">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="73"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="72"/>
+      <c r="A12" s="74"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="65"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="72">
+      <c r="B13" s="66"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="65">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="74"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="72"/>
+      <c r="A14" s="66"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="65"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="40"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="33"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6081,10 +6081,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="60" t="s">
+      <c r="E25" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="60"/>
+      <c r="F25" s="56"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6099,8 +6099,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6116,10 +6116,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="34">
+      <c r="E27" s="36">
         <v>30</v>
       </c>
-      <c r="F27" s="34"/>
+      <c r="F27" s="36"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6135,8 +6135,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6152,10 +6152,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="34">
+      <c r="E29" s="36">
         <v>5</v>
       </c>
-      <c r="F29" s="34"/>
+      <c r="F29" s="36"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6171,8 +6171,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6188,10 +6188,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="59">
+      <c r="E31" s="60">
         <v>2</v>
       </c>
-      <c r="F31" s="59"/>
+      <c r="F31" s="60"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6254,58 +6254,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="43" t="s">
+      <c r="A36" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="43"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="43" t="s">
+      <c r="H36" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="36"/>
-      <c r="B37" s="36"/>
+      <c r="A37" s="35"/>
+      <c r="B37" s="35"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="36"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="36"/>
-      <c r="B38" s="36"/>
+      <c r="A38" s="35"/>
+      <c r="B38" s="35"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="36"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="35"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="36"/>
-      <c r="B39" s="36"/>
+      <c r="A39" s="35"/>
+      <c r="B39" s="35"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="36" t="s">
+      <c r="H39" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="43"/>
-      <c r="J39" s="43"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6315,29 +6315,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="38"/>
-      <c r="I40" s="39"/>
-      <c r="J40" s="39"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6354,6 +6337,23 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
07.08.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/August/Others/Cash.xlsx
+++ b/August/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 05.08.19</t>
+    <t>Date: 07.08.19</t>
   </si>
 </sst>
 </file>
@@ -473,12 +473,39 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -488,90 +515,63 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -579,12 +579,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -606,6 +600,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2054,7 +2054,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2076,60 +2076,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2138,10 +2138,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2156,10 +2156,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>50</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2175,10 +2175,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>16</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2194,10 +2194,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>151</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2213,10 +2213,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="34">
         <v>58</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2232,8 +2232,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2249,8 +2249,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2263,10 +2263,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2313,58 +2313,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2374,11 +2374,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2453,60 +2453,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2515,10 +2515,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="41"/>
+      <c r="F31" s="30"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2533,10 +2533,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="34">
         <v>50</v>
       </c>
-      <c r="F32" s="36"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2552,10 +2552,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>116</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2571,10 +2571,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>151</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2590,10 +2590,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="34">
         <v>58</v>
       </c>
-      <c r="F35" s="36"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2609,8 +2609,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2626,8 +2626,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2640,10 +2640,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="32" t="s">
+      <c r="D38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="33"/>
+      <c r="E38" s="42"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2690,58 +2690,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2751,11 +2751,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2783,6 +2783,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2795,32 +2821,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2832,8 +2832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="H46" sqref="A1:J46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2851,63 +2851,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2917,10 +2917,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="48"/>
+      <c r="F5" s="53"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2935,13 +2935,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="44">
-        <v>64</v>
-      </c>
-      <c r="F6" s="44"/>
+      <c r="E6" s="54">
+        <v>49</v>
+      </c>
+      <c r="F6" s="54"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>64000</v>
+        <v>49000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2954,13 +2954,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="44">
-        <v>108</v>
-      </c>
-      <c r="F7" s="44"/>
+      <c r="E7" s="54">
+        <v>189</v>
+      </c>
+      <c r="F7" s="54"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>54000</v>
+        <v>94500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2973,13 +2973,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="44">
-        <v>180</v>
-      </c>
-      <c r="F8" s="44"/>
+      <c r="E8" s="54">
+        <v>229</v>
+      </c>
+      <c r="F8" s="54"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>18000</v>
+        <v>22900</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2992,11 +2992,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
+      <c r="E9" s="54">
+        <v>64</v>
+      </c>
+      <c r="F9" s="54"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3200</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3009,13 +3011,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="44">
-        <v>200</v>
-      </c>
-      <c r="F10" s="44"/>
+      <c r="E10" s="54">
+        <v>12</v>
+      </c>
+      <c r="F10" s="54"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>240</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3028,11 +3030,13 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
+      <c r="E11" s="54">
+        <v>116</v>
+      </c>
+      <c r="F11" s="54"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1160</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3042,14 +3046,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="51"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>140000</v>
+        <v>171000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3092,58 +3096,58 @@
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="49"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="49" t="s">
+      <c r="H16" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="46"/>
+      <c r="B17" s="46"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="49"/>
-      <c r="B19" s="49"/>
+      <c r="A19" s="46"/>
+      <c r="B19" s="46"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="50" t="s">
+      <c r="H19" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="26"/>
@@ -3153,9 +3157,9 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="26"/>
@@ -3242,60 +3246,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="51"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="52"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="47" t="s">
+      <c r="A31" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="47"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3304,10 +3308,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="48" t="s">
+      <c r="E32" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="48"/>
+      <c r="F32" s="53"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3322,13 +3326,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="44">
-        <v>64</v>
-      </c>
-      <c r="F33" s="44"/>
+      <c r="E33" s="54">
+        <v>49</v>
+      </c>
+      <c r="F33" s="54"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>64000</v>
+        <v>49000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3341,13 +3345,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="44">
-        <v>108</v>
-      </c>
-      <c r="F34" s="44"/>
+      <c r="E34" s="54">
+        <v>189</v>
+      </c>
+      <c r="F34" s="54"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>54000</v>
+        <v>94500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3360,13 +3364,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="44">
-        <v>180</v>
-      </c>
-      <c r="F35" s="44"/>
+      <c r="E35" s="54">
+        <v>229</v>
+      </c>
+      <c r="F35" s="54"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>18000</v>
+        <v>22900</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3379,11 +3383,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="44"/>
-      <c r="F36" s="44"/>
+      <c r="E36" s="54">
+        <v>64</v>
+      </c>
+      <c r="F36" s="54"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3200</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3396,13 +3402,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="44">
-        <v>200</v>
-      </c>
-      <c r="F37" s="44"/>
+      <c r="E37" s="54">
+        <v>12</v>
+      </c>
+      <c r="F37" s="54"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>4000</v>
+        <v>240</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3415,11 +3421,13 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="44"/>
-      <c r="F38" s="44"/>
+      <c r="E38" s="54">
+        <v>116</v>
+      </c>
+      <c r="F38" s="54"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1160</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3429,14 +3437,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="54" t="s">
+      <c r="D39" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="55"/>
+      <c r="E39" s="49"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>140000</v>
+        <v>171000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3479,58 +3487,58 @@
       <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="49" t="s">
+      <c r="A43" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="49"/>
+      <c r="B43" s="46"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="49" t="s">
+      <c r="H43" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="49"/>
-      <c r="J43" s="49"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="46"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="53"/>
-      <c r="B44" s="53"/>
+      <c r="A44" s="45"/>
+      <c r="B44" s="45"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="53"/>
-      <c r="I44" s="53"/>
-      <c r="J44" s="53"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
+      <c r="J44" s="45"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="53"/>
-      <c r="B45" s="53"/>
+      <c r="A45" s="45"/>
+      <c r="B45" s="45"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="53"/>
-      <c r="I45" s="53"/>
-      <c r="J45" s="53"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="45"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
-      <c r="A46" s="49"/>
-      <c r="B46" s="49"/>
+      <c r="A46" s="46"/>
+      <c r="B46" s="46"/>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="50" t="s">
+      <c r="H46" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="50"/>
-      <c r="J46" s="50"/>
+      <c r="I46" s="47"/>
+      <c r="J46" s="47"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3540,9 +3548,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3570,6 +3578,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3586,28 +3616,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3638,63 +3646,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3704,10 +3712,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3722,10 +3730,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>68</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3741,10 +3749,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>135</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3760,10 +3768,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>53</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3779,10 +3787,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="34">
         <v>2</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3798,10 +3806,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="36">
+      <c r="E10" s="34">
         <v>5</v>
       </c>
-      <c r="F10" s="36"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3817,8 +3825,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3831,10 +3839,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3881,76 +3889,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="35"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="57"/>
+      <c r="B20" s="56"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4025,60 +4033,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4087,10 +4095,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="56" t="s">
+      <c r="E31" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="56"/>
+      <c r="F31" s="60"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4105,10 +4113,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="60">
+      <c r="E32" s="59">
         <v>68</v>
       </c>
-      <c r="F32" s="60"/>
+      <c r="F32" s="59"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4124,10 +4132,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="60">
+      <c r="E33" s="59">
         <v>135</v>
       </c>
-      <c r="F33" s="60"/>
+      <c r="F33" s="59"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4143,10 +4151,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="60">
+      <c r="E34" s="59">
         <v>53</v>
       </c>
-      <c r="F34" s="60"/>
+      <c r="F34" s="59"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4162,10 +4170,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="60">
+      <c r="E35" s="59">
         <v>2</v>
       </c>
-      <c r="F35" s="60"/>
+      <c r="F35" s="59"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4181,10 +4189,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="60">
+      <c r="E36" s="59">
         <v>5</v>
       </c>
-      <c r="F36" s="60"/>
+      <c r="F36" s="59"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4200,8 +4208,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4214,10 +4222,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="59" t="s">
+      <c r="D38" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="59"/>
+      <c r="E38" s="58"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4264,76 +4272,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="35"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58" t="s">
+      <c r="A46" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="58"/>
+      <c r="B46" s="57"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4361,6 +4369,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4377,30 +4409,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4432,63 +4440,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4498,10 +4506,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4516,10 +4524,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>44</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4535,10 +4543,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>118</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4554,10 +4562,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>510</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4573,8 +4581,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4590,8 +4598,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4607,8 +4615,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4621,10 +4629,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4671,72 +4679,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="61"/>
-      <c r="B20" s="61"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="62"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4811,60 +4819,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4873,10 +4881,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="41"/>
+      <c r="F31" s="30"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4891,10 +4899,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="34">
         <v>44</v>
       </c>
-      <c r="F32" s="36"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4910,10 +4918,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>118</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4929,10 +4937,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>510</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4948,8 +4956,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4965,8 +4973,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4982,8 +4990,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4996,10 +5004,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="62" t="s">
+      <c r="D38" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="62"/>
+      <c r="E38" s="61"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5046,72 +5054,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58"/>
-      <c r="B46" s="58"/>
+      <c r="A46" s="57"/>
+      <c r="B46" s="57"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5139,16 +5147,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5161,24 +5177,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5203,64 +5211,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5271,8 +5279,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5283,8 +5291,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5295,8 +5303,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5307,8 +5315,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5319,8 +5327,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5331,8 +5339,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5342,8 +5350,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5387,52 +5395,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42"/>
-      <c r="B16" s="42"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5442,9 +5450,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5531,60 +5539,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5595,10 +5603,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="56" t="s">
+      <c r="E32" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="56"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5613,10 +5621,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>30</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5632,10 +5640,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>35</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5651,10 +5659,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="34">
         <v>425</v>
       </c>
-      <c r="F35" s="36"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5670,8 +5678,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5687,8 +5695,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5704,10 +5712,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="60">
+      <c r="E38" s="59">
         <v>100</v>
       </c>
-      <c r="F38" s="60"/>
+      <c r="F38" s="59"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5770,58 +5778,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="34"/>
+      <c r="B43" s="43"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="34" t="s">
+      <c r="H43" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="35"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="36"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="35"/>
-      <c r="B46" s="35"/>
+      <c r="A46" s="36"/>
+      <c r="B46" s="36"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
+      <c r="I46" s="43"/>
+      <c r="J46" s="43"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5831,12 +5839,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5849,32 +5883,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5900,177 +5908,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="74">
+      <c r="A5" s="73">
         <v>1</v>
       </c>
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="65">
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="72">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="74"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="65"/>
+      <c r="A6" s="73"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="72"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="74">
+      <c r="A7" s="73">
         <v>2</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="65">
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="72">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="74"/>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="65"/>
+      <c r="A8" s="73"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="72"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="74">
+      <c r="A9" s="73">
         <v>3</v>
       </c>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="65">
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="72">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="74"/>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="65"/>
+      <c r="A10" s="73"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="72"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="74">
+      <c r="A11" s="73">
         <v>4</v>
       </c>
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="65">
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="72">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="74"/>
-      <c r="B12" s="71"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="65"/>
+      <c r="A12" s="73"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="72"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="66" t="s">
+      <c r="A13" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="65">
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="72">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="66"/>
-      <c r="B14" s="66"/>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="65"/>
+      <c r="A14" s="74"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="72"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="40"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6081,10 +6089,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="56" t="s">
+      <c r="E25" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="56"/>
+      <c r="F25" s="60"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6099,8 +6107,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6116,10 +6124,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="36">
+      <c r="E27" s="34">
         <v>30</v>
       </c>
-      <c r="F27" s="36"/>
+      <c r="F27" s="34"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6135,8 +6143,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6152,10 +6160,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="36">
+      <c r="E29" s="34">
         <v>5</v>
       </c>
-      <c r="F29" s="36"/>
+      <c r="F29" s="34"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6171,8 +6179,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="59"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6188,10 +6196,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="60">
+      <c r="E31" s="59">
         <v>2</v>
       </c>
-      <c r="F31" s="60"/>
+      <c r="F31" s="59"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6254,58 +6262,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="34"/>
+      <c r="B36" s="43"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="34" t="s">
+      <c r="H36" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="35"/>
-      <c r="B37" s="35"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="36"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="35"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="36"/>
+      <c r="J37" s="36"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="35"/>
-      <c r="B38" s="35"/>
+      <c r="A38" s="36"/>
+      <c r="B38" s="36"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="35"/>
-      <c r="J38" s="35"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="36"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="35"/>
-      <c r="B39" s="35"/>
+      <c r="A39" s="36"/>
+      <c r="B39" s="36"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="35" t="s">
+      <c r="H39" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
+      <c r="I39" s="43"/>
+      <c r="J39" s="43"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6315,12 +6323,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="31"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6337,23 +6362,6 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
09.08.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/August/Others/Cash.xlsx
+++ b/August/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 08.08.19</t>
+    <t>Date: 09.08.19</t>
   </si>
 </sst>
 </file>
@@ -473,47 +473,71 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -521,34 +545,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -563,15 +566,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -579,6 +579,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -600,12 +606,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2054,7 +2054,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2076,60 +2076,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2138,10 +2138,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2156,10 +2156,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>50</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2175,10 +2175,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>16</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2194,10 +2194,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>151</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2213,10 +2213,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="36">
         <v>58</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2232,8 +2232,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2249,8 +2249,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2263,10 +2263,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2313,58 +2313,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2374,11 +2374,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2453,60 +2453,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2515,10 +2515,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="30"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2533,10 +2533,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="36">
         <v>50</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="36"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2552,10 +2552,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>116</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2571,10 +2571,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>151</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2590,10 +2590,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="36">
         <v>58</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2609,8 +2609,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2626,8 +2626,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2640,10 +2640,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="41" t="s">
+      <c r="D38" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="42"/>
+      <c r="E38" s="33"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2690,58 +2690,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2751,11 +2751,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2783,14 +2783,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2803,24 +2813,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2851,63 +2851,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2917,10 +2917,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="53"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2935,13 +2935,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="54">
-        <v>61</v>
-      </c>
-      <c r="F6" s="54"/>
+      <c r="E6" s="44">
+        <v>100</v>
+      </c>
+      <c r="F6" s="44"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>61000</v>
+        <v>100000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2954,13 +2954,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="54">
-        <v>124</v>
-      </c>
-      <c r="F7" s="54"/>
+      <c r="E7" s="44">
+        <v>149</v>
+      </c>
+      <c r="F7" s="44"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>62000</v>
+        <v>74500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2973,13 +2973,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="54">
-        <v>179</v>
-      </c>
-      <c r="F8" s="54"/>
+      <c r="E8" s="44">
+        <v>205</v>
+      </c>
+      <c r="F8" s="44"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>17900</v>
+        <v>20500</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2992,13 +2992,11 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="54">
-        <v>10</v>
-      </c>
-      <c r="F9" s="54"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3011,13 +3009,11 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="54">
-        <v>225</v>
-      </c>
-      <c r="F10" s="54"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>4500</v>
+        <v>0</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3030,13 +3026,11 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="54">
-        <v>10</v>
-      </c>
-      <c r="F11" s="54"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3046,14 +3040,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="55"/>
+      <c r="E12" s="51"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>146000</v>
+        <v>195000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3096,58 +3090,58 @@
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="46"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="46" t="s">
+      <c r="H16" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="46"/>
-      <c r="B17" s="46"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="46"/>
-      <c r="B18" s="46"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="46"/>
-      <c r="B19" s="46"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="47" t="s">
+      <c r="H19" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="26"/>
@@ -3157,9 +3151,9 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="26"/>
@@ -3246,60 +3240,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="50"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="50"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="51"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="52" t="s">
+      <c r="A30" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="52"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="52"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="52" t="s">
+      <c r="A31" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="52"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="52"/>
-      <c r="I31" s="52"/>
-      <c r="J31" s="52"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3308,10 +3302,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="53" t="s">
+      <c r="E32" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="53"/>
+      <c r="F32" s="48"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3326,13 +3320,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="54">
-        <v>61</v>
-      </c>
-      <c r="F33" s="54"/>
+      <c r="E33" s="44">
+        <v>100</v>
+      </c>
+      <c r="F33" s="44"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>61000</v>
+        <v>100000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3345,13 +3339,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="54">
-        <v>124</v>
-      </c>
-      <c r="F34" s="54"/>
+      <c r="E34" s="44">
+        <v>149</v>
+      </c>
+      <c r="F34" s="44"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>62000</v>
+        <v>74500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3364,13 +3358,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="54">
-        <v>179</v>
-      </c>
-      <c r="F35" s="54"/>
+      <c r="E35" s="44">
+        <v>205</v>
+      </c>
+      <c r="F35" s="44"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>17900</v>
+        <v>20500</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3383,13 +3377,11 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="54">
-        <v>10</v>
-      </c>
-      <c r="F36" s="54"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="44"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3402,13 +3394,11 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="54">
-        <v>225</v>
-      </c>
-      <c r="F37" s="54"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>4500</v>
+        <v>0</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3421,13 +3411,11 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="54">
-        <v>10</v>
-      </c>
-      <c r="F38" s="54"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="44"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3437,14 +3425,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="48" t="s">
+      <c r="D39" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="49"/>
+      <c r="E39" s="55"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>146000</v>
+        <v>195000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3487,58 +3475,58 @@
       <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="46" t="s">
+      <c r="A43" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="46"/>
+      <c r="B43" s="49"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="46" t="s">
+      <c r="H43" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="46"/>
-      <c r="J43" s="46"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="45"/>
-      <c r="B44" s="45"/>
+      <c r="A44" s="53"/>
+      <c r="B44" s="53"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="45"/>
-      <c r="I44" s="45"/>
-      <c r="J44" s="45"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="53"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="45"/>
-      <c r="B45" s="45"/>
+      <c r="A45" s="53"/>
+      <c r="B45" s="53"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="45"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="53"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
-      <c r="A46" s="46"/>
-      <c r="B46" s="46"/>
+      <c r="A46" s="49"/>
+      <c r="B46" s="49"/>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="47" t="s">
+      <c r="H46" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="47"/>
-      <c r="J46" s="47"/>
+      <c r="I46" s="50"/>
+      <c r="J46" s="50"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3548,9 +3536,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3578,28 +3566,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3616,6 +3582,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3646,63 +3634,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3712,10 +3700,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3730,10 +3718,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>68</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3749,10 +3737,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>135</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3768,10 +3756,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>53</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3787,10 +3775,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="36">
         <v>2</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3806,10 +3794,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="36">
         <v>5</v>
       </c>
-      <c r="F10" s="34"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3825,8 +3813,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3839,10 +3827,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3889,76 +3877,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="36"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="56" t="s">
+      <c r="A20" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="56"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4033,60 +4021,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4095,10 +4083,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="60" t="s">
+      <c r="E31" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="60"/>
+      <c r="F31" s="56"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4113,10 +4101,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="59">
+      <c r="E32" s="60">
         <v>68</v>
       </c>
-      <c r="F32" s="59"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4132,10 +4120,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="59">
+      <c r="E33" s="60">
         <v>135</v>
       </c>
-      <c r="F33" s="59"/>
+      <c r="F33" s="60"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4151,10 +4139,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="59">
+      <c r="E34" s="60">
         <v>53</v>
       </c>
-      <c r="F34" s="59"/>
+      <c r="F34" s="60"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4170,10 +4158,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="59">
+      <c r="E35" s="60">
         <v>2</v>
       </c>
-      <c r="F35" s="59"/>
+      <c r="F35" s="60"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4189,10 +4177,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="59">
+      <c r="E36" s="60">
         <v>5</v>
       </c>
-      <c r="F36" s="59"/>
+      <c r="F36" s="60"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4208,8 +4196,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4222,10 +4210,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="58" t="s">
+      <c r="D38" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="58"/>
+      <c r="E38" s="59"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4272,76 +4260,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="36" t="s">
+      <c r="A45" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="36"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="57" t="s">
+      <c r="A46" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="57"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4369,30 +4357,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4409,6 +4373,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4440,63 +4428,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4506,10 +4494,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4524,10 +4512,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>44</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4543,10 +4531,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>118</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4562,10 +4550,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>510</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4581,8 +4569,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4598,8 +4586,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4615,8 +4603,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4629,10 +4617,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4679,72 +4667,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="62"/>
-      <c r="B20" s="62"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="61"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4819,60 +4807,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4881,10 +4869,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="30"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4899,10 +4887,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="36">
         <v>44</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="36"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4918,10 +4906,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>118</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4937,10 +4925,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>510</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4956,8 +4944,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4973,8 +4961,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4990,8 +4978,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5004,10 +4992,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="61" t="s">
+      <c r="D38" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="61"/>
+      <c r="E38" s="62"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5054,72 +5042,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="57"/>
-      <c r="B46" s="57"/>
+      <c r="A46" s="58"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5147,6 +5135,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5159,34 +5175,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5211,64 +5199,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5279,8 +5267,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5291,8 +5279,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5303,8 +5291,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5315,8 +5303,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5327,8 +5315,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5339,8 +5327,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5350,8 +5338,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5395,52 +5383,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5450,9 +5438,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5539,60 +5527,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5603,10 +5591,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="60" t="s">
+      <c r="E32" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="60"/>
+      <c r="F32" s="56"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5621,10 +5609,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>30</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5640,10 +5628,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>35</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5659,10 +5647,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="36">
         <v>425</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5678,8 +5666,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5695,8 +5683,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5712,10 +5700,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="59">
+      <c r="E38" s="60">
         <v>100</v>
       </c>
-      <c r="F38" s="59"/>
+      <c r="F38" s="60"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5778,58 +5766,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="43"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="43" t="s">
+      <c r="H43" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="36"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="36"/>
-      <c r="B46" s="36"/>
+      <c r="A46" s="35"/>
+      <c r="B46" s="35"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="36" t="s">
+      <c r="H46" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="43"/>
-      <c r="J46" s="43"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5839,20 +5827,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -5865,24 +5863,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5908,177 +5896,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="73">
+      <c r="A5" s="74">
         <v>1</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="72">
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="65">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="73"/>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="72"/>
+      <c r="A6" s="74"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="65"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="73">
+      <c r="A7" s="74">
         <v>2</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="72">
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="65">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="73"/>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="72"/>
+      <c r="A8" s="74"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="65"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="73">
+      <c r="A9" s="74">
         <v>3</v>
       </c>
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="72">
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="65">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="73"/>
-      <c r="B10" s="65"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="72"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="65"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="73">
+      <c r="A11" s="74">
         <v>4</v>
       </c>
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="72">
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="65">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="73"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="72"/>
+      <c r="A12" s="74"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="65"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="72">
+      <c r="B13" s="66"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="65">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="74"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="72"/>
+      <c r="A14" s="66"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="65"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="40"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="33"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6089,10 +6077,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="60" t="s">
+      <c r="E25" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="60"/>
+      <c r="F25" s="56"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6107,8 +6095,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6124,10 +6112,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="34">
+      <c r="E27" s="36">
         <v>30</v>
       </c>
-      <c r="F27" s="34"/>
+      <c r="F27" s="36"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6143,8 +6131,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6160,10 +6148,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="34">
+      <c r="E29" s="36">
         <v>5</v>
       </c>
-      <c r="F29" s="34"/>
+      <c r="F29" s="36"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6179,8 +6167,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6196,10 +6184,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="59">
+      <c r="E31" s="60">
         <v>2</v>
       </c>
-      <c r="F31" s="59"/>
+      <c r="F31" s="60"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6262,58 +6250,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="43" t="s">
+      <c r="A36" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="43"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="43" t="s">
+      <c r="H36" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="36"/>
-      <c r="B37" s="36"/>
+      <c r="A37" s="35"/>
+      <c r="B37" s="35"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="36"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="36"/>
-      <c r="B38" s="36"/>
+      <c r="A38" s="35"/>
+      <c r="B38" s="35"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="36"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="35"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="36"/>
-      <c r="B39" s="36"/>
+      <c r="A39" s="35"/>
+      <c r="B39" s="35"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="36" t="s">
+      <c r="H39" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="43"/>
-      <c r="J39" s="43"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6323,29 +6311,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="38"/>
-      <c r="I40" s="39"/>
-      <c r="J40" s="39"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6362,6 +6333,23 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
10.08.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/August/Others/Cash.xlsx
+++ b/August/Others/Cash.xlsx
@@ -473,12 +473,39 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -488,90 +515,63 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -579,12 +579,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -606,6 +600,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2054,7 +2054,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2076,60 +2076,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2138,10 +2138,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2156,10 +2156,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>50</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2175,10 +2175,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>16</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2194,10 +2194,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>151</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2213,10 +2213,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="34">
         <v>58</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2232,8 +2232,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2249,8 +2249,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2263,10 +2263,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2313,58 +2313,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2374,11 +2374,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2453,60 +2453,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2515,10 +2515,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="41"/>
+      <c r="F31" s="30"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2533,10 +2533,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="34">
         <v>50</v>
       </c>
-      <c r="F32" s="36"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2552,10 +2552,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>116</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2571,10 +2571,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>151</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2590,10 +2590,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="34">
         <v>58</v>
       </c>
-      <c r="F35" s="36"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2609,8 +2609,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2626,8 +2626,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2640,10 +2640,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="32" t="s">
+      <c r="D38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="33"/>
+      <c r="E38" s="42"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2690,58 +2690,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2751,11 +2751,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2783,6 +2783,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2795,32 +2821,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2833,7 +2833,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H46" sqref="A1:J46"/>
+      <selection activeCell="N5" sqref="N4:O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2851,63 +2851,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2917,10 +2917,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="48"/>
+      <c r="F5" s="53"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2935,10 +2935,10 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="44">
+      <c r="E6" s="54">
         <v>100</v>
       </c>
-      <c r="F6" s="44"/>
+      <c r="F6" s="54"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>100000</v>
@@ -2954,10 +2954,10 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="44">
+      <c r="E7" s="54">
         <v>149</v>
       </c>
-      <c r="F7" s="44"/>
+      <c r="F7" s="54"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
         <v>74500</v>
@@ -2973,10 +2973,10 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="44">
+      <c r="E8" s="54">
         <v>205</v>
       </c>
-      <c r="F8" s="44"/>
+      <c r="F8" s="54"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
         <v>20500</v>
@@ -2992,8 +2992,8 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3009,8 +3009,8 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3026,8 +3026,8 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3040,10 +3040,10 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="51"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
@@ -3090,58 +3090,58 @@
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="49"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="49" t="s">
+      <c r="H16" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="46"/>
+      <c r="B17" s="46"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="49"/>
-      <c r="B19" s="49"/>
+      <c r="A19" s="46"/>
+      <c r="B19" s="46"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="50" t="s">
+      <c r="H19" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="26"/>
@@ -3151,9 +3151,9 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="26"/>
@@ -3240,60 +3240,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="51"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="52"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="47" t="s">
+      <c r="A31" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="47"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3302,10 +3302,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="48" t="s">
+      <c r="E32" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="48"/>
+      <c r="F32" s="53"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3320,10 +3320,10 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="44">
+      <c r="E33" s="54">
         <v>100</v>
       </c>
-      <c r="F33" s="44"/>
+      <c r="F33" s="54"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
         <v>100000</v>
@@ -3339,10 +3339,10 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="44">
+      <c r="E34" s="54">
         <v>149</v>
       </c>
-      <c r="F34" s="44"/>
+      <c r="F34" s="54"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
         <v>74500</v>
@@ -3358,10 +3358,10 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="44">
+      <c r="E35" s="54">
         <v>205</v>
       </c>
-      <c r="F35" s="44"/>
+      <c r="F35" s="54"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
         <v>20500</v>
@@ -3377,8 +3377,8 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="44"/>
-      <c r="F36" s="44"/>
+      <c r="E36" s="54"/>
+      <c r="F36" s="54"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3394,8 +3394,8 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="54"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -3411,8 +3411,8 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="44"/>
-      <c r="F38" s="44"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="54"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3425,10 +3425,10 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="54" t="s">
+      <c r="D39" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="55"/>
+      <c r="E39" s="49"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
@@ -3475,58 +3475,58 @@
       <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="49" t="s">
+      <c r="A43" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="49"/>
+      <c r="B43" s="46"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="49" t="s">
+      <c r="H43" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="49"/>
-      <c r="J43" s="49"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="46"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="53"/>
-      <c r="B44" s="53"/>
+      <c r="A44" s="45"/>
+      <c r="B44" s="45"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="53"/>
-      <c r="I44" s="53"/>
-      <c r="J44" s="53"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
+      <c r="J44" s="45"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="53"/>
-      <c r="B45" s="53"/>
+      <c r="A45" s="45"/>
+      <c r="B45" s="45"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="53"/>
-      <c r="I45" s="53"/>
-      <c r="J45" s="53"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="45"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
-      <c r="A46" s="49"/>
-      <c r="B46" s="49"/>
+      <c r="A46" s="46"/>
+      <c r="B46" s="46"/>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="50" t="s">
+      <c r="H46" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="50"/>
-      <c r="J46" s="50"/>
+      <c r="I46" s="47"/>
+      <c r="J46" s="47"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3536,9 +3536,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3566,6 +3566,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3582,28 +3604,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3634,63 +3634,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3700,10 +3700,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3718,10 +3718,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>68</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3737,10 +3737,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>135</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3756,10 +3756,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>53</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3775,10 +3775,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="34">
         <v>2</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3794,10 +3794,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="36">
+      <c r="E10" s="34">
         <v>5</v>
       </c>
-      <c r="F10" s="36"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3813,8 +3813,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3827,10 +3827,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3877,76 +3877,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="35"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="57"/>
+      <c r="B20" s="56"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4021,60 +4021,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4083,10 +4083,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="56" t="s">
+      <c r="E31" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="56"/>
+      <c r="F31" s="60"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4101,10 +4101,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="60">
+      <c r="E32" s="59">
         <v>68</v>
       </c>
-      <c r="F32" s="60"/>
+      <c r="F32" s="59"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4120,10 +4120,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="60">
+      <c r="E33" s="59">
         <v>135</v>
       </c>
-      <c r="F33" s="60"/>
+      <c r="F33" s="59"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4139,10 +4139,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="60">
+      <c r="E34" s="59">
         <v>53</v>
       </c>
-      <c r="F34" s="60"/>
+      <c r="F34" s="59"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4158,10 +4158,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="60">
+      <c r="E35" s="59">
         <v>2</v>
       </c>
-      <c r="F35" s="60"/>
+      <c r="F35" s="59"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4177,10 +4177,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="60">
+      <c r="E36" s="59">
         <v>5</v>
       </c>
-      <c r="F36" s="60"/>
+      <c r="F36" s="59"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4196,8 +4196,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4210,10 +4210,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="59" t="s">
+      <c r="D38" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="59"/>
+      <c r="E38" s="58"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4260,76 +4260,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="35"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58" t="s">
+      <c r="A46" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="58"/>
+      <c r="B46" s="57"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4357,6 +4357,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4373,30 +4397,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4428,63 +4428,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4494,10 +4494,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4512,10 +4512,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>44</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4531,10 +4531,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>118</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4550,10 +4550,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>510</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4569,8 +4569,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4586,8 +4586,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4603,8 +4603,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4617,10 +4617,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4667,72 +4667,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="61"/>
-      <c r="B20" s="61"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="62"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4807,60 +4807,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4869,10 +4869,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="41"/>
+      <c r="F31" s="30"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4887,10 +4887,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="34">
         <v>44</v>
       </c>
-      <c r="F32" s="36"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4906,10 +4906,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>118</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4925,10 +4925,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>510</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4944,8 +4944,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4961,8 +4961,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4978,8 +4978,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4992,10 +4992,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="62" t="s">
+      <c r="D38" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="62"/>
+      <c r="E38" s="61"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5042,72 +5042,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58"/>
-      <c r="B46" s="58"/>
+      <c r="A46" s="57"/>
+      <c r="B46" s="57"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5135,16 +5135,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5157,24 +5165,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5199,64 +5199,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5267,8 +5267,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5279,8 +5279,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5291,8 +5291,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5303,8 +5303,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5315,8 +5315,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5327,8 +5327,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5338,8 +5338,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5383,52 +5383,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42"/>
-      <c r="B16" s="42"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5438,9 +5438,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5527,60 +5527,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5591,10 +5591,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="56" t="s">
+      <c r="E32" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="56"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5609,10 +5609,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>30</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5628,10 +5628,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>35</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5647,10 +5647,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="34">
         <v>425</v>
       </c>
-      <c r="F35" s="36"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5666,8 +5666,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5683,8 +5683,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5700,10 +5700,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="60">
+      <c r="E38" s="59">
         <v>100</v>
       </c>
-      <c r="F38" s="60"/>
+      <c r="F38" s="59"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5766,58 +5766,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="34"/>
+      <c r="B43" s="43"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="34" t="s">
+      <c r="H43" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="35"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="36"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="35"/>
-      <c r="B46" s="35"/>
+      <c r="A46" s="36"/>
+      <c r="B46" s="36"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
+      <c r="I46" s="43"/>
+      <c r="J46" s="43"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5827,12 +5827,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5845,32 +5871,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5896,177 +5896,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="74">
+      <c r="A5" s="73">
         <v>1</v>
       </c>
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="65">
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="72">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="74"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="65"/>
+      <c r="A6" s="73"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="72"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="74">
+      <c r="A7" s="73">
         <v>2</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="65">
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="72">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="74"/>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="65"/>
+      <c r="A8" s="73"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="72"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="74">
+      <c r="A9" s="73">
         <v>3</v>
       </c>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="65">
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="72">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="74"/>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="65"/>
+      <c r="A10" s="73"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="72"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="74">
+      <c r="A11" s="73">
         <v>4</v>
       </c>
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="65">
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="72">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="74"/>
-      <c r="B12" s="71"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="65"/>
+      <c r="A12" s="73"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="72"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="66" t="s">
+      <c r="A13" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="65">
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="72">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="66"/>
-      <c r="B14" s="66"/>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="65"/>
+      <c r="A14" s="74"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="72"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="40"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6077,10 +6077,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="56" t="s">
+      <c r="E25" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="56"/>
+      <c r="F25" s="60"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6095,8 +6095,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6112,10 +6112,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="36">
+      <c r="E27" s="34">
         <v>30</v>
       </c>
-      <c r="F27" s="36"/>
+      <c r="F27" s="34"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6131,8 +6131,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6148,10 +6148,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="36">
+      <c r="E29" s="34">
         <v>5</v>
       </c>
-      <c r="F29" s="36"/>
+      <c r="F29" s="34"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6167,8 +6167,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="59"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6184,10 +6184,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="60">
+      <c r="E31" s="59">
         <v>2</v>
       </c>
-      <c r="F31" s="60"/>
+      <c r="F31" s="59"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6250,58 +6250,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="34"/>
+      <c r="B36" s="43"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="34" t="s">
+      <c r="H36" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="35"/>
-      <c r="B37" s="35"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="36"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="35"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="36"/>
+      <c r="J37" s="36"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="35"/>
-      <c r="B38" s="35"/>
+      <c r="A38" s="36"/>
+      <c r="B38" s="36"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="35"/>
-      <c r="J38" s="35"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="36"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="35"/>
-      <c r="B39" s="35"/>
+      <c r="A39" s="36"/>
+      <c r="B39" s="36"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="35" t="s">
+      <c r="H39" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
+      <c r="I39" s="43"/>
+      <c r="J39" s="43"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6311,12 +6311,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="31"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6333,23 +6350,6 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
11.08.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/August/Others/Cash.xlsx
+++ b/August/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 09.08.19</t>
+    <t>Date: 11.08.19</t>
   </si>
 </sst>
 </file>
@@ -473,47 +473,71 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -521,34 +545,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -563,15 +566,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -579,6 +579,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -600,12 +606,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2054,7 +2054,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2076,60 +2076,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2138,10 +2138,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2156,10 +2156,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>50</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2175,10 +2175,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>16</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2194,10 +2194,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>151</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2213,10 +2213,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="36">
         <v>58</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2232,8 +2232,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2249,8 +2249,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2263,10 +2263,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2313,58 +2313,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2374,11 +2374,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2453,60 +2453,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2515,10 +2515,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="30"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2533,10 +2533,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="36">
         <v>50</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="36"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2552,10 +2552,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>116</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2571,10 +2571,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>151</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2590,10 +2590,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="36">
         <v>58</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2609,8 +2609,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2626,8 +2626,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2640,10 +2640,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="41" t="s">
+      <c r="D38" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="42"/>
+      <c r="E38" s="33"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2690,58 +2690,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2751,11 +2751,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2783,14 +2783,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2803,24 +2813,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2833,7 +2833,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N4:O5"/>
+      <selection activeCell="H46" sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2851,63 +2851,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2917,10 +2917,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="53"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2935,13 +2935,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="54">
-        <v>100</v>
-      </c>
-      <c r="F6" s="54"/>
+      <c r="E6" s="44">
+        <v>73</v>
+      </c>
+      <c r="F6" s="44"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>100000</v>
+        <v>73000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2954,13 +2954,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="54">
-        <v>149</v>
-      </c>
-      <c r="F7" s="54"/>
+      <c r="E7" s="44">
+        <v>244</v>
+      </c>
+      <c r="F7" s="44"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>74500</v>
+        <v>122000</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2973,13 +2973,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="54">
-        <v>205</v>
-      </c>
-      <c r="F8" s="54"/>
+      <c r="E8" s="44">
+        <v>100</v>
+      </c>
+      <c r="F8" s="44"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>20500</v>
+        <v>10000</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2992,8 +2992,8 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3009,8 +3009,8 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3026,8 +3026,8 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3040,14 +3040,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="55"/>
+      <c r="E12" s="51"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>195000</v>
+        <v>205000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3090,58 +3090,58 @@
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="46"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="46" t="s">
+      <c r="H16" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="46"/>
-      <c r="B17" s="46"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="46"/>
-      <c r="B18" s="46"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="46"/>
-      <c r="B19" s="46"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="47" t="s">
+      <c r="H19" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="26"/>
@@ -3151,9 +3151,9 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="26"/>
@@ -3240,60 +3240,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="50"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="50"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="51"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="52" t="s">
+      <c r="A30" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="52"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="52"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="52" t="s">
+      <c r="A31" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="52"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="52"/>
-      <c r="I31" s="52"/>
-      <c r="J31" s="52"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3302,10 +3302,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="53" t="s">
+      <c r="E32" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="53"/>
+      <c r="F32" s="48"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3320,13 +3320,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="54">
-        <v>100</v>
-      </c>
-      <c r="F33" s="54"/>
+      <c r="E33" s="44">
+        <v>73</v>
+      </c>
+      <c r="F33" s="44"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>100000</v>
+        <v>73000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3339,13 +3339,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="54">
-        <v>149</v>
-      </c>
-      <c r="F34" s="54"/>
+      <c r="E34" s="44">
+        <v>244</v>
+      </c>
+      <c r="F34" s="44"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>74500</v>
+        <v>122000</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3358,13 +3358,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="54">
-        <v>205</v>
-      </c>
-      <c r="F35" s="54"/>
+      <c r="E35" s="44">
+        <v>100</v>
+      </c>
+      <c r="F35" s="44"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>20500</v>
+        <v>10000</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3377,8 +3377,8 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="54"/>
-      <c r="F36" s="54"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="44"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3394,8 +3394,8 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -3411,8 +3411,8 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="54"/>
-      <c r="F38" s="54"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="44"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3425,14 +3425,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="48" t="s">
+      <c r="D39" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="49"/>
+      <c r="E39" s="55"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>195000</v>
+        <v>205000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3475,58 +3475,58 @@
       <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="46" t="s">
+      <c r="A43" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="46"/>
+      <c r="B43" s="49"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="46" t="s">
+      <c r="H43" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="46"/>
-      <c r="J43" s="46"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="45"/>
-      <c r="B44" s="45"/>
+      <c r="A44" s="53"/>
+      <c r="B44" s="53"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="45"/>
-      <c r="I44" s="45"/>
-      <c r="J44" s="45"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="53"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="45"/>
-      <c r="B45" s="45"/>
+      <c r="A45" s="53"/>
+      <c r="B45" s="53"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="45"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="53"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
-      <c r="A46" s="46"/>
-      <c r="B46" s="46"/>
+      <c r="A46" s="49"/>
+      <c r="B46" s="49"/>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="47" t="s">
+      <c r="H46" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="47"/>
-      <c r="J46" s="47"/>
+      <c r="I46" s="50"/>
+      <c r="J46" s="50"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3536,9 +3536,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3566,28 +3566,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3604,6 +3582,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3634,63 +3634,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3700,10 +3700,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3718,10 +3718,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>68</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3737,10 +3737,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>135</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3756,10 +3756,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>53</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3775,10 +3775,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="36">
         <v>2</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3794,10 +3794,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="36">
         <v>5</v>
       </c>
-      <c r="F10" s="34"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3813,8 +3813,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3827,10 +3827,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3877,76 +3877,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="36"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="56" t="s">
+      <c r="A20" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="56"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4021,60 +4021,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4083,10 +4083,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="60" t="s">
+      <c r="E31" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="60"/>
+      <c r="F31" s="56"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4101,10 +4101,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="59">
+      <c r="E32" s="60">
         <v>68</v>
       </c>
-      <c r="F32" s="59"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4120,10 +4120,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="59">
+      <c r="E33" s="60">
         <v>135</v>
       </c>
-      <c r="F33" s="59"/>
+      <c r="F33" s="60"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4139,10 +4139,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="59">
+      <c r="E34" s="60">
         <v>53</v>
       </c>
-      <c r="F34" s="59"/>
+      <c r="F34" s="60"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4158,10 +4158,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="59">
+      <c r="E35" s="60">
         <v>2</v>
       </c>
-      <c r="F35" s="59"/>
+      <c r="F35" s="60"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4177,10 +4177,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="59">
+      <c r="E36" s="60">
         <v>5</v>
       </c>
-      <c r="F36" s="59"/>
+      <c r="F36" s="60"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4196,8 +4196,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4210,10 +4210,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="58" t="s">
+      <c r="D38" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="58"/>
+      <c r="E38" s="59"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4260,76 +4260,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="36" t="s">
+      <c r="A45" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="36"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="57" t="s">
+      <c r="A46" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="57"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4357,30 +4357,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4397,6 +4373,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4428,63 +4428,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4494,10 +4494,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4512,10 +4512,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>44</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4531,10 +4531,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>118</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4550,10 +4550,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>510</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4569,8 +4569,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4586,8 +4586,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4603,8 +4603,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4617,10 +4617,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4667,72 +4667,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="62"/>
-      <c r="B20" s="62"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="61"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4807,60 +4807,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4869,10 +4869,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="30"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4887,10 +4887,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="36">
         <v>44</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="36"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4906,10 +4906,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>118</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4925,10 +4925,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>510</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4944,8 +4944,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4961,8 +4961,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4978,8 +4978,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4992,10 +4992,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="61" t="s">
+      <c r="D38" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="61"/>
+      <c r="E38" s="62"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5042,72 +5042,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="57"/>
-      <c r="B46" s="57"/>
+      <c r="A46" s="58"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5135,6 +5135,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5147,34 +5175,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5199,64 +5199,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5267,8 +5267,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5279,8 +5279,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5291,8 +5291,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5303,8 +5303,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5315,8 +5315,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5327,8 +5327,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5338,8 +5338,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5383,52 +5383,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5438,9 +5438,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5527,60 +5527,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5591,10 +5591,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="60" t="s">
+      <c r="E32" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="60"/>
+      <c r="F32" s="56"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5609,10 +5609,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>30</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5628,10 +5628,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>35</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5647,10 +5647,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="36">
         <v>425</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5666,8 +5666,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5683,8 +5683,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5700,10 +5700,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="59">
+      <c r="E38" s="60">
         <v>100</v>
       </c>
-      <c r="F38" s="59"/>
+      <c r="F38" s="60"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5766,58 +5766,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="43"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="43" t="s">
+      <c r="H43" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="36"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="36"/>
-      <c r="B46" s="36"/>
+      <c r="A46" s="35"/>
+      <c r="B46" s="35"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="36" t="s">
+      <c r="H46" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="43"/>
-      <c r="J46" s="43"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5827,20 +5827,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -5853,24 +5863,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5896,177 +5896,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="73">
+      <c r="A5" s="74">
         <v>1</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="72">
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="65">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="73"/>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="72"/>
+      <c r="A6" s="74"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="65"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="73">
+      <c r="A7" s="74">
         <v>2</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="72">
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="65">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="73"/>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="72"/>
+      <c r="A8" s="74"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="65"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="73">
+      <c r="A9" s="74">
         <v>3</v>
       </c>
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="72">
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="65">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="73"/>
-      <c r="B10" s="65"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="72"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="65"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="73">
+      <c r="A11" s="74">
         <v>4</v>
       </c>
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="72">
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="65">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="73"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="72"/>
+      <c r="A12" s="74"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="65"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="72">
+      <c r="B13" s="66"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="65">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="74"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="72"/>
+      <c r="A14" s="66"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="65"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="40"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="33"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6077,10 +6077,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="60" t="s">
+      <c r="E25" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="60"/>
+      <c r="F25" s="56"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6095,8 +6095,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6112,10 +6112,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="34">
+      <c r="E27" s="36">
         <v>30</v>
       </c>
-      <c r="F27" s="34"/>
+      <c r="F27" s="36"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6131,8 +6131,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6148,10 +6148,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="34">
+      <c r="E29" s="36">
         <v>5</v>
       </c>
-      <c r="F29" s="34"/>
+      <c r="F29" s="36"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6167,8 +6167,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6184,10 +6184,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="59">
+      <c r="E31" s="60">
         <v>2</v>
       </c>
-      <c r="F31" s="59"/>
+      <c r="F31" s="60"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6250,58 +6250,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="43" t="s">
+      <c r="A36" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="43"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="43" t="s">
+      <c r="H36" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="36"/>
-      <c r="B37" s="36"/>
+      <c r="A37" s="35"/>
+      <c r="B37" s="35"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="36"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="36"/>
-      <c r="B38" s="36"/>
+      <c r="A38" s="35"/>
+      <c r="B38" s="35"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="36"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="35"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="36"/>
-      <c r="B39" s="36"/>
+      <c r="A39" s="35"/>
+      <c r="B39" s="35"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="36" t="s">
+      <c r="H39" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="43"/>
-      <c r="J39" s="43"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6311,29 +6311,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="38"/>
-      <c r="I40" s="39"/>
-      <c r="J40" s="39"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6350,6 +6333,23 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
17.08.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/August/Others/Cash.xlsx
+++ b/August/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 11.08.19</t>
+    <t>Date: 17.08.19</t>
   </si>
 </sst>
 </file>
@@ -2832,8 +2832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H46" sqref="A1:J46"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2936,12 +2936,12 @@
         <v>1000</v>
       </c>
       <c r="E6" s="44">
-        <v>73</v>
+        <v>158</v>
       </c>
       <c r="F6" s="44"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>73000</v>
+        <v>158000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2955,12 +2955,12 @@
         <v>500</v>
       </c>
       <c r="E7" s="44">
-        <v>244</v>
+        <v>487</v>
       </c>
       <c r="F7" s="44"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>122000</v>
+        <v>243500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2974,12 +2974,12 @@
         <v>100</v>
       </c>
       <c r="E8" s="44">
-        <v>100</v>
+        <v>565</v>
       </c>
       <c r="F8" s="44"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>10000</v>
+        <v>56500</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -3047,7 +3047,7 @@
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>205000</v>
+        <v>458000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3321,12 +3321,12 @@
         <v>1000</v>
       </c>
       <c r="E33" s="44">
-        <v>73</v>
+        <v>158</v>
       </c>
       <c r="F33" s="44"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>73000</v>
+        <v>158000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3340,12 +3340,12 @@
         <v>500</v>
       </c>
       <c r="E34" s="44">
-        <v>244</v>
+        <v>487</v>
       </c>
       <c r="F34" s="44"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>122000</v>
+        <v>243500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3359,12 +3359,12 @@
         <v>100</v>
       </c>
       <c r="E35" s="44">
-        <v>100</v>
+        <v>565</v>
       </c>
       <c r="F35" s="44"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>56500</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3432,7 +3432,7 @@
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>205000</v>
+        <v>458000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>

</xml_diff>

<commit_message>
19.08.19 Today Sales Detailsa
</commit_message>
<xml_diff>
--- a/August/Others/Cash.xlsx
+++ b/August/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 17.08.19</t>
+    <t>Date: 19.08.19</t>
   </si>
 </sst>
 </file>
@@ -2832,8 +2832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection sqref="A1:J46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H46" sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2936,12 +2936,12 @@
         <v>1000</v>
       </c>
       <c r="E6" s="44">
-        <v>158</v>
+        <v>53</v>
       </c>
       <c r="F6" s="44"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>158000</v>
+        <v>53000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2955,12 +2955,12 @@
         <v>500</v>
       </c>
       <c r="E7" s="44">
-        <v>487</v>
+        <v>201</v>
       </c>
       <c r="F7" s="44"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>243500</v>
+        <v>100500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2974,12 +2974,12 @@
         <v>100</v>
       </c>
       <c r="E8" s="44">
-        <v>565</v>
+        <v>159</v>
       </c>
       <c r="F8" s="44"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>56500</v>
+        <v>15900</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2992,11 +2992,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="44"/>
+      <c r="E9" s="44">
+        <v>18</v>
+      </c>
       <c r="F9" s="44"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3009,11 +3011,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="44"/>
+      <c r="E10" s="44">
+        <v>118</v>
+      </c>
       <c r="F10" s="44"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2360</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3026,11 +3030,13 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="44"/>
+      <c r="E11" s="44">
+        <v>234</v>
+      </c>
       <c r="F11" s="44"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2340</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3047,7 +3053,7 @@
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>458000</v>
+        <v>175000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3321,12 +3327,12 @@
         <v>1000</v>
       </c>
       <c r="E33" s="44">
-        <v>158</v>
+        <v>53</v>
       </c>
       <c r="F33" s="44"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>158000</v>
+        <v>53000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3340,12 +3346,12 @@
         <v>500</v>
       </c>
       <c r="E34" s="44">
-        <v>487</v>
+        <v>201</v>
       </c>
       <c r="F34" s="44"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>243500</v>
+        <v>100500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3359,12 +3365,12 @@
         <v>100</v>
       </c>
       <c r="E35" s="44">
-        <v>565</v>
+        <v>159</v>
       </c>
       <c r="F35" s="44"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>56500</v>
+        <v>15900</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3377,11 +3383,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="44"/>
+      <c r="E36" s="44">
+        <v>18</v>
+      </c>
       <c r="F36" s="44"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>900</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3394,11 +3402,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="44"/>
+      <c r="E37" s="44">
+        <v>118</v>
+      </c>
       <c r="F37" s="44"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>0</v>
+        <v>2360</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3411,11 +3421,13 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="44"/>
+      <c r="E38" s="44">
+        <v>234</v>
+      </c>
       <c r="F38" s="44"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2340</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3432,7 +3444,7 @@
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>458000</v>
+        <v>175000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>

</xml_diff>

<commit_message>
20.08.19 today Sales Details
</commit_message>
<xml_diff>
--- a/August/Others/Cash.xlsx
+++ b/August/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 19.08.19</t>
+    <t>Date: 20.08.19</t>
   </si>
 </sst>
 </file>
@@ -473,12 +473,39 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -488,90 +515,63 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -579,12 +579,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -606,6 +600,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2054,7 +2054,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2076,60 +2076,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2138,10 +2138,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2156,10 +2156,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>50</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2175,10 +2175,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>16</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2194,10 +2194,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>151</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2213,10 +2213,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="34">
         <v>58</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2232,8 +2232,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2249,8 +2249,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2263,10 +2263,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2313,58 +2313,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2374,11 +2374,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2453,60 +2453,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2515,10 +2515,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="41"/>
+      <c r="F31" s="30"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2533,10 +2533,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="34">
         <v>50</v>
       </c>
-      <c r="F32" s="36"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2552,10 +2552,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>116</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2571,10 +2571,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>151</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2590,10 +2590,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="34">
         <v>58</v>
       </c>
-      <c r="F35" s="36"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2609,8 +2609,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2626,8 +2626,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2640,10 +2640,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="32" t="s">
+      <c r="D38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="33"/>
+      <c r="E38" s="42"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2690,58 +2690,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2751,11 +2751,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2783,6 +2783,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2795,32 +2821,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2851,63 +2851,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2917,10 +2917,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="48"/>
+      <c r="F5" s="53"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2935,13 +2935,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="44">
-        <v>53</v>
-      </c>
-      <c r="F6" s="44"/>
+      <c r="E6" s="54">
+        <v>46</v>
+      </c>
+      <c r="F6" s="54"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>53000</v>
+        <v>46000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2954,13 +2954,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="44">
-        <v>201</v>
-      </c>
-      <c r="F7" s="44"/>
+      <c r="E7" s="54">
+        <v>111</v>
+      </c>
+      <c r="F7" s="54"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>100500</v>
+        <v>55500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2973,13 +2973,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="44">
-        <v>159</v>
-      </c>
-      <c r="F8" s="44"/>
+      <c r="E8" s="54">
+        <v>51</v>
+      </c>
+      <c r="F8" s="54"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>15900</v>
+        <v>5100</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2992,13 +2992,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="44">
-        <v>18</v>
-      </c>
-      <c r="F9" s="44"/>
+      <c r="E9" s="54">
+        <v>86</v>
+      </c>
+      <c r="F9" s="54"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>4300</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3011,13 +3011,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="44">
-        <v>118</v>
-      </c>
-      <c r="F10" s="44"/>
+      <c r="E10" s="54">
+        <v>100</v>
+      </c>
+      <c r="F10" s="54"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>2360</v>
+        <v>2000</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3030,13 +3030,13 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="44">
-        <v>234</v>
-      </c>
-      <c r="F11" s="44"/>
+      <c r="E11" s="54">
+        <v>110</v>
+      </c>
+      <c r="F11" s="54"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>2340</v>
+        <v>1100</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3046,14 +3046,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="51"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>175000</v>
+        <v>114000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3096,58 +3096,58 @@
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="49"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="49" t="s">
+      <c r="H16" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="46"/>
+      <c r="B17" s="46"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="49"/>
-      <c r="B19" s="49"/>
+      <c r="A19" s="46"/>
+      <c r="B19" s="46"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="50" t="s">
+      <c r="H19" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="26"/>
@@ -3157,9 +3157,9 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="26"/>
@@ -3246,60 +3246,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="51"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="52"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="47" t="s">
+      <c r="A31" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="47"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3308,10 +3308,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="48" t="s">
+      <c r="E32" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="48"/>
+      <c r="F32" s="53"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3326,13 +3326,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="44">
-        <v>53</v>
-      </c>
-      <c r="F33" s="44"/>
+      <c r="E33" s="54">
+        <v>46</v>
+      </c>
+      <c r="F33" s="54"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>53000</v>
+        <v>46000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3345,13 +3345,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="44">
-        <v>201</v>
-      </c>
-      <c r="F34" s="44"/>
+      <c r="E34" s="54">
+        <v>111</v>
+      </c>
+      <c r="F34" s="54"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>100500</v>
+        <v>55500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3364,13 +3364,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="44">
-        <v>159</v>
-      </c>
-      <c r="F35" s="44"/>
+      <c r="E35" s="54">
+        <v>51</v>
+      </c>
+      <c r="F35" s="54"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>15900</v>
+        <v>5100</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3383,13 +3383,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="44">
-        <v>18</v>
-      </c>
-      <c r="F36" s="44"/>
+      <c r="E36" s="54">
+        <v>86</v>
+      </c>
+      <c r="F36" s="54"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>900</v>
+        <v>4300</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3402,13 +3402,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="44">
-        <v>118</v>
-      </c>
-      <c r="F37" s="44"/>
+      <c r="E37" s="54">
+        <v>100</v>
+      </c>
+      <c r="F37" s="54"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>2360</v>
+        <v>2000</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3421,13 +3421,13 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="44">
-        <v>234</v>
-      </c>
-      <c r="F38" s="44"/>
+      <c r="E38" s="54">
+        <v>110</v>
+      </c>
+      <c r="F38" s="54"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>2340</v>
+        <v>1100</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3437,14 +3437,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="54" t="s">
+      <c r="D39" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="55"/>
+      <c r="E39" s="49"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>175000</v>
+        <v>114000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3487,58 +3487,58 @@
       <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="49" t="s">
+      <c r="A43" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="49"/>
+      <c r="B43" s="46"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="49" t="s">
+      <c r="H43" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="49"/>
-      <c r="J43" s="49"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="46"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="53"/>
-      <c r="B44" s="53"/>
+      <c r="A44" s="45"/>
+      <c r="B44" s="45"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="53"/>
-      <c r="I44" s="53"/>
-      <c r="J44" s="53"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
+      <c r="J44" s="45"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="53"/>
-      <c r="B45" s="53"/>
+      <c r="A45" s="45"/>
+      <c r="B45" s="45"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="53"/>
-      <c r="I45" s="53"/>
-      <c r="J45" s="53"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="45"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
-      <c r="A46" s="49"/>
-      <c r="B46" s="49"/>
+      <c r="A46" s="46"/>
+      <c r="B46" s="46"/>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="50" t="s">
+      <c r="H46" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="50"/>
-      <c r="J46" s="50"/>
+      <c r="I46" s="47"/>
+      <c r="J46" s="47"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3548,9 +3548,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3578,6 +3578,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3594,28 +3616,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3646,63 +3646,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3712,10 +3712,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3730,10 +3730,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>68</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3749,10 +3749,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>135</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3768,10 +3768,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>53</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3787,10 +3787,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="34">
         <v>2</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3806,10 +3806,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="36">
+      <c r="E10" s="34">
         <v>5</v>
       </c>
-      <c r="F10" s="36"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3825,8 +3825,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3839,10 +3839,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3889,76 +3889,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="35"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="57"/>
+      <c r="B20" s="56"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4033,60 +4033,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4095,10 +4095,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="56" t="s">
+      <c r="E31" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="56"/>
+      <c r="F31" s="60"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4113,10 +4113,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="60">
+      <c r="E32" s="59">
         <v>68</v>
       </c>
-      <c r="F32" s="60"/>
+      <c r="F32" s="59"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4132,10 +4132,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="60">
+      <c r="E33" s="59">
         <v>135</v>
       </c>
-      <c r="F33" s="60"/>
+      <c r="F33" s="59"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4151,10 +4151,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="60">
+      <c r="E34" s="59">
         <v>53</v>
       </c>
-      <c r="F34" s="60"/>
+      <c r="F34" s="59"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4170,10 +4170,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="60">
+      <c r="E35" s="59">
         <v>2</v>
       </c>
-      <c r="F35" s="60"/>
+      <c r="F35" s="59"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4189,10 +4189,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="60">
+      <c r="E36" s="59">
         <v>5</v>
       </c>
-      <c r="F36" s="60"/>
+      <c r="F36" s="59"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4208,8 +4208,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4222,10 +4222,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="59" t="s">
+      <c r="D38" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="59"/>
+      <c r="E38" s="58"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4272,76 +4272,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="35"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58" t="s">
+      <c r="A46" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="58"/>
+      <c r="B46" s="57"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4369,6 +4369,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4385,30 +4409,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4440,63 +4440,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4506,10 +4506,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4524,10 +4524,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>44</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4543,10 +4543,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>118</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4562,10 +4562,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>510</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4581,8 +4581,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4598,8 +4598,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4615,8 +4615,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4629,10 +4629,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4679,72 +4679,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="61"/>
-      <c r="B20" s="61"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="62"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4819,60 +4819,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4881,10 +4881,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="41"/>
+      <c r="F31" s="30"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4899,10 +4899,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="34">
         <v>44</v>
       </c>
-      <c r="F32" s="36"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4918,10 +4918,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>118</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4937,10 +4937,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>510</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4956,8 +4956,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4973,8 +4973,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4990,8 +4990,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5004,10 +5004,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="62" t="s">
+      <c r="D38" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="62"/>
+      <c r="E38" s="61"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5054,72 +5054,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58"/>
-      <c r="B46" s="58"/>
+      <c r="A46" s="57"/>
+      <c r="B46" s="57"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5147,16 +5147,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5169,24 +5177,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5211,64 +5211,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5279,8 +5279,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5291,8 +5291,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5303,8 +5303,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5315,8 +5315,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5327,8 +5327,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5339,8 +5339,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5350,8 +5350,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5395,52 +5395,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42"/>
-      <c r="B16" s="42"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5450,9 +5450,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5539,60 +5539,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5603,10 +5603,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="56" t="s">
+      <c r="E32" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="56"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5621,10 +5621,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>30</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5640,10 +5640,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>35</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5659,10 +5659,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="34">
         <v>425</v>
       </c>
-      <c r="F35" s="36"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5678,8 +5678,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5695,8 +5695,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5712,10 +5712,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="60">
+      <c r="E38" s="59">
         <v>100</v>
       </c>
-      <c r="F38" s="60"/>
+      <c r="F38" s="59"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5778,58 +5778,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="34"/>
+      <c r="B43" s="43"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="34" t="s">
+      <c r="H43" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="35"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="36"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="35"/>
-      <c r="B46" s="35"/>
+      <c r="A46" s="36"/>
+      <c r="B46" s="36"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
+      <c r="I46" s="43"/>
+      <c r="J46" s="43"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5839,12 +5839,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5857,32 +5883,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5908,177 +5908,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="74">
+      <c r="A5" s="73">
         <v>1</v>
       </c>
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="65">
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="72">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="74"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="65"/>
+      <c r="A6" s="73"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="72"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="74">
+      <c r="A7" s="73">
         <v>2</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="65">
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="72">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="74"/>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="65"/>
+      <c r="A8" s="73"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="72"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="74">
+      <c r="A9" s="73">
         <v>3</v>
       </c>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="65">
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="72">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="74"/>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="65"/>
+      <c r="A10" s="73"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="72"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="74">
+      <c r="A11" s="73">
         <v>4</v>
       </c>
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="65">
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="72">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="74"/>
-      <c r="B12" s="71"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="65"/>
+      <c r="A12" s="73"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="72"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="66" t="s">
+      <c r="A13" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="65">
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="72">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="66"/>
-      <c r="B14" s="66"/>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="65"/>
+      <c r="A14" s="74"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="72"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="40"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6089,10 +6089,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="56" t="s">
+      <c r="E25" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="56"/>
+      <c r="F25" s="60"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6107,8 +6107,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6124,10 +6124,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="36">
+      <c r="E27" s="34">
         <v>30</v>
       </c>
-      <c r="F27" s="36"/>
+      <c r="F27" s="34"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6143,8 +6143,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6160,10 +6160,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="36">
+      <c r="E29" s="34">
         <v>5</v>
       </c>
-      <c r="F29" s="36"/>
+      <c r="F29" s="34"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6179,8 +6179,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="59"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6196,10 +6196,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="60">
+      <c r="E31" s="59">
         <v>2</v>
       </c>
-      <c r="F31" s="60"/>
+      <c r="F31" s="59"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6262,58 +6262,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="34"/>
+      <c r="B36" s="43"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="34" t="s">
+      <c r="H36" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="35"/>
-      <c r="B37" s="35"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="36"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="35"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="36"/>
+      <c r="J37" s="36"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="35"/>
-      <c r="B38" s="35"/>
+      <c r="A38" s="36"/>
+      <c r="B38" s="36"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="35"/>
-      <c r="J38" s="35"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="36"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="35"/>
-      <c r="B39" s="35"/>
+      <c r="A39" s="36"/>
+      <c r="B39" s="36"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="35" t="s">
+      <c r="H39" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
+      <c r="I39" s="43"/>
+      <c r="J39" s="43"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6323,12 +6323,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="31"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6345,23 +6362,6 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
22.08.19 today Sales Details
</commit_message>
<xml_diff>
--- a/August/Others/Cash.xlsx
+++ b/August/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 20.08.19</t>
+    <t>Date: 22.08.19</t>
   </si>
 </sst>
 </file>
@@ -2936,12 +2936,12 @@
         <v>1000</v>
       </c>
       <c r="E6" s="54">
-        <v>46</v>
+        <v>122</v>
       </c>
       <c r="F6" s="54"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>46000</v>
+        <v>122000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2955,12 +2955,12 @@
         <v>500</v>
       </c>
       <c r="E7" s="54">
-        <v>111</v>
+        <v>315</v>
       </c>
       <c r="F7" s="54"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>55500</v>
+        <v>157500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2974,12 +2974,12 @@
         <v>100</v>
       </c>
       <c r="E8" s="54">
-        <v>51</v>
+        <v>200</v>
       </c>
       <c r="F8" s="54"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>5100</v>
+        <v>20000</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2992,13 +2992,11 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="54">
-        <v>86</v>
-      </c>
+      <c r="E9" s="54"/>
       <c r="F9" s="54"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>4300</v>
+        <v>0</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3012,12 +3010,12 @@
         <v>20</v>
       </c>
       <c r="E10" s="54">
-        <v>100</v>
+        <v>165</v>
       </c>
       <c r="F10" s="54"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>3300</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3031,12 +3029,12 @@
         <v>10</v>
       </c>
       <c r="E11" s="54">
-        <v>110</v>
+        <v>20</v>
       </c>
       <c r="F11" s="54"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>1100</v>
+        <v>200</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3053,7 +3051,7 @@
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>114000</v>
+        <v>303000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3327,12 +3325,12 @@
         <v>1000</v>
       </c>
       <c r="E33" s="54">
-        <v>46</v>
+        <v>122</v>
       </c>
       <c r="F33" s="54"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>46000</v>
+        <v>122000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3346,12 +3344,12 @@
         <v>500</v>
       </c>
       <c r="E34" s="54">
-        <v>111</v>
+        <v>315</v>
       </c>
       <c r="F34" s="54"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>55500</v>
+        <v>157500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3365,12 +3363,12 @@
         <v>100</v>
       </c>
       <c r="E35" s="54">
-        <v>51</v>
+        <v>200</v>
       </c>
       <c r="F35" s="54"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>5100</v>
+        <v>20000</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3383,13 +3381,11 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="54">
-        <v>86</v>
-      </c>
+      <c r="E36" s="54"/>
       <c r="F36" s="54"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>4300</v>
+        <v>0</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3403,12 +3399,12 @@
         <v>20</v>
       </c>
       <c r="E37" s="54">
-        <v>100</v>
+        <v>165</v>
       </c>
       <c r="F37" s="54"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>2000</v>
+        <v>3300</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3422,12 +3418,12 @@
         <v>10</v>
       </c>
       <c r="E38" s="54">
-        <v>110</v>
+        <v>20</v>
       </c>
       <c r="F38" s="54"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>1100</v>
+        <v>200</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3444,7 +3440,7 @@
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>114000</v>
+        <v>303000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>

</xml_diff>

<commit_message>
24.08.19 today Sales details
</commit_message>
<xml_diff>
--- a/August/Others/Cash.xlsx
+++ b/August/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 22.08.19</t>
+    <t>Date: 24.08.19</t>
   </si>
 </sst>
 </file>
@@ -473,47 +473,71 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -521,34 +545,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -563,15 +566,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -579,6 +579,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -600,12 +606,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2054,7 +2054,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2076,60 +2076,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2138,10 +2138,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2156,10 +2156,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>50</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2175,10 +2175,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>16</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2194,10 +2194,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>151</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2213,10 +2213,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="36">
         <v>58</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2232,8 +2232,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2249,8 +2249,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2263,10 +2263,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2313,58 +2313,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2374,11 +2374,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2453,60 +2453,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2515,10 +2515,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="30"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2533,10 +2533,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="36">
         <v>50</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="36"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2552,10 +2552,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>116</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2571,10 +2571,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>151</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2590,10 +2590,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="36">
         <v>58</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2609,8 +2609,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2626,8 +2626,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2640,10 +2640,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="41" t="s">
+      <c r="D38" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="42"/>
+      <c r="E38" s="33"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2690,58 +2690,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2751,11 +2751,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2783,14 +2783,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2803,24 +2813,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2851,63 +2851,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2917,10 +2917,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="53"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2935,13 +2935,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="54">
-        <v>122</v>
-      </c>
-      <c r="F6" s="54"/>
+      <c r="E6" s="44">
+        <v>78</v>
+      </c>
+      <c r="F6" s="44"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>122000</v>
+        <v>78000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2954,13 +2954,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="54">
-        <v>315</v>
-      </c>
-      <c r="F7" s="54"/>
+      <c r="E7" s="44">
+        <v>114</v>
+      </c>
+      <c r="F7" s="44"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>157500</v>
+        <v>57000</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2973,13 +2973,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="54">
-        <v>200</v>
-      </c>
-      <c r="F8" s="54"/>
+      <c r="E8" s="44">
+        <v>290</v>
+      </c>
+      <c r="F8" s="44"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>20000</v>
+        <v>29000</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2992,8 +2992,8 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3009,13 +3009,11 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="54">
-        <v>165</v>
-      </c>
-      <c r="F10" s="54"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>3300</v>
+        <v>0</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3028,13 +3026,11 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="54">
-        <v>20</v>
-      </c>
-      <c r="F11" s="54"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3044,14 +3040,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="55"/>
+      <c r="E12" s="51"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>303000</v>
+        <v>164000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3094,58 +3090,58 @@
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="46"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="46" t="s">
+      <c r="H16" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="46"/>
-      <c r="B17" s="46"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="46"/>
-      <c r="B18" s="46"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="46"/>
-      <c r="B19" s="46"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="47" t="s">
+      <c r="H19" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="26"/>
@@ -3155,9 +3151,9 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="26"/>
@@ -3244,60 +3240,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="50"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="50"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="51"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="52" t="s">
+      <c r="A30" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="52"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="52"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="52" t="s">
+      <c r="A31" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="52"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="52"/>
-      <c r="I31" s="52"/>
-      <c r="J31" s="52"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3306,10 +3302,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="53" t="s">
+      <c r="E32" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="53"/>
+      <c r="F32" s="48"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3324,13 +3320,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="54">
-        <v>122</v>
-      </c>
-      <c r="F33" s="54"/>
+      <c r="E33" s="44">
+        <v>78</v>
+      </c>
+      <c r="F33" s="44"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>122000</v>
+        <v>78000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3343,13 +3339,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="54">
-        <v>315</v>
-      </c>
-      <c r="F34" s="54"/>
+      <c r="E34" s="44">
+        <v>114</v>
+      </c>
+      <c r="F34" s="44"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>157500</v>
+        <v>57000</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3362,13 +3358,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="54">
-        <v>200</v>
-      </c>
-      <c r="F35" s="54"/>
+      <c r="E35" s="44">
+        <v>290</v>
+      </c>
+      <c r="F35" s="44"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>20000</v>
+        <v>29000</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3381,8 +3377,8 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="54"/>
-      <c r="F36" s="54"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="44"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3398,13 +3394,11 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="54">
-        <v>165</v>
-      </c>
-      <c r="F37" s="54"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>3300</v>
+        <v>0</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3417,13 +3411,11 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="54">
-        <v>20</v>
-      </c>
-      <c r="F38" s="54"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="44"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3433,14 +3425,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="48" t="s">
+      <c r="D39" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="49"/>
+      <c r="E39" s="55"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>303000</v>
+        <v>164000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3483,58 +3475,58 @@
       <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="46" t="s">
+      <c r="A43" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="46"/>
+      <c r="B43" s="49"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="46" t="s">
+      <c r="H43" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="46"/>
-      <c r="J43" s="46"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="45"/>
-      <c r="B44" s="45"/>
+      <c r="A44" s="53"/>
+      <c r="B44" s="53"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="45"/>
-      <c r="I44" s="45"/>
-      <c r="J44" s="45"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="53"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="45"/>
-      <c r="B45" s="45"/>
+      <c r="A45" s="53"/>
+      <c r="B45" s="53"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="45"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="53"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
-      <c r="A46" s="46"/>
-      <c r="B46" s="46"/>
+      <c r="A46" s="49"/>
+      <c r="B46" s="49"/>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="47" t="s">
+      <c r="H46" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="47"/>
-      <c r="J46" s="47"/>
+      <c r="I46" s="50"/>
+      <c r="J46" s="50"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3544,9 +3536,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3574,28 +3566,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3612,6 +3582,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3642,63 +3634,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3708,10 +3700,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3726,10 +3718,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>68</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3745,10 +3737,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>135</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3764,10 +3756,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>53</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3783,10 +3775,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="36">
         <v>2</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3802,10 +3794,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="36">
         <v>5</v>
       </c>
-      <c r="F10" s="34"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3821,8 +3813,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3835,10 +3827,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3885,76 +3877,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="36"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="56" t="s">
+      <c r="A20" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="56"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4029,60 +4021,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4091,10 +4083,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="60" t="s">
+      <c r="E31" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="60"/>
+      <c r="F31" s="56"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4109,10 +4101,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="59">
+      <c r="E32" s="60">
         <v>68</v>
       </c>
-      <c r="F32" s="59"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4128,10 +4120,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="59">
+      <c r="E33" s="60">
         <v>135</v>
       </c>
-      <c r="F33" s="59"/>
+      <c r="F33" s="60"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4147,10 +4139,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="59">
+      <c r="E34" s="60">
         <v>53</v>
       </c>
-      <c r="F34" s="59"/>
+      <c r="F34" s="60"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4166,10 +4158,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="59">
+      <c r="E35" s="60">
         <v>2</v>
       </c>
-      <c r="F35" s="59"/>
+      <c r="F35" s="60"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4185,10 +4177,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="59">
+      <c r="E36" s="60">
         <v>5</v>
       </c>
-      <c r="F36" s="59"/>
+      <c r="F36" s="60"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4204,8 +4196,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4218,10 +4210,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="58" t="s">
+      <c r="D38" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="58"/>
+      <c r="E38" s="59"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4268,76 +4260,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="36" t="s">
+      <c r="A45" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="36"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="57" t="s">
+      <c r="A46" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="57"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4365,30 +4357,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4405,6 +4373,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4436,63 +4428,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4502,10 +4494,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4520,10 +4512,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>44</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4539,10 +4531,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>118</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4558,10 +4550,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>510</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4577,8 +4569,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4594,8 +4586,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4611,8 +4603,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4625,10 +4617,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4675,72 +4667,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="62"/>
-      <c r="B20" s="62"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="61"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4815,60 +4807,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4877,10 +4869,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="30"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4895,10 +4887,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="36">
         <v>44</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="36"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4914,10 +4906,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>118</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4933,10 +4925,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>510</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4952,8 +4944,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4969,8 +4961,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4986,8 +4978,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5000,10 +4992,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="61" t="s">
+      <c r="D38" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="61"/>
+      <c r="E38" s="62"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5050,72 +5042,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="57"/>
-      <c r="B46" s="57"/>
+      <c r="A46" s="58"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5143,6 +5135,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5155,34 +5175,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5207,64 +5199,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5275,8 +5267,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5287,8 +5279,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5299,8 +5291,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5311,8 +5303,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5323,8 +5315,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5335,8 +5327,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5346,8 +5338,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5391,52 +5383,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5446,9 +5438,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5535,60 +5527,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5599,10 +5591,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="60" t="s">
+      <c r="E32" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="60"/>
+      <c r="F32" s="56"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5617,10 +5609,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>30</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5636,10 +5628,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>35</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5655,10 +5647,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="36">
         <v>425</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5674,8 +5666,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5691,8 +5683,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5708,10 +5700,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="59">
+      <c r="E38" s="60">
         <v>100</v>
       </c>
-      <c r="F38" s="59"/>
+      <c r="F38" s="60"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5774,58 +5766,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="43"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="43" t="s">
+      <c r="H43" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="36"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="36"/>
-      <c r="B46" s="36"/>
+      <c r="A46" s="35"/>
+      <c r="B46" s="35"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="36" t="s">
+      <c r="H46" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="43"/>
-      <c r="J46" s="43"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5835,20 +5827,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -5861,24 +5863,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5904,177 +5896,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="73">
+      <c r="A5" s="74">
         <v>1</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="72">
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="65">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="73"/>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="72"/>
+      <c r="A6" s="74"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="65"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="73">
+      <c r="A7" s="74">
         <v>2</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="72">
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="65">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="73"/>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="72"/>
+      <c r="A8" s="74"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="65"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="73">
+      <c r="A9" s="74">
         <v>3</v>
       </c>
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="72">
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="65">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="73"/>
-      <c r="B10" s="65"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="72"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="65"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="73">
+      <c r="A11" s="74">
         <v>4</v>
       </c>
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="72">
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="65">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="73"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="72"/>
+      <c r="A12" s="74"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="65"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="72">
+      <c r="B13" s="66"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="65">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="74"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="72"/>
+      <c r="A14" s="66"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="65"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="40"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="33"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6085,10 +6077,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="60" t="s">
+      <c r="E25" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="60"/>
+      <c r="F25" s="56"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6103,8 +6095,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6120,10 +6112,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="34">
+      <c r="E27" s="36">
         <v>30</v>
       </c>
-      <c r="F27" s="34"/>
+      <c r="F27" s="36"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6139,8 +6131,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6156,10 +6148,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="34">
+      <c r="E29" s="36">
         <v>5</v>
       </c>
-      <c r="F29" s="34"/>
+      <c r="F29" s="36"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6175,8 +6167,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6192,10 +6184,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="59">
+      <c r="E31" s="60">
         <v>2</v>
       </c>
-      <c r="F31" s="59"/>
+      <c r="F31" s="60"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6258,58 +6250,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="43" t="s">
+      <c r="A36" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="43"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="43" t="s">
+      <c r="H36" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="36"/>
-      <c r="B37" s="36"/>
+      <c r="A37" s="35"/>
+      <c r="B37" s="35"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="36"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="36"/>
-      <c r="B38" s="36"/>
+      <c r="A38" s="35"/>
+      <c r="B38" s="35"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="36"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="35"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="36"/>
-      <c r="B39" s="36"/>
+      <c r="A39" s="35"/>
+      <c r="B39" s="35"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="36" t="s">
+      <c r="H39" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="43"/>
-      <c r="J39" s="43"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6319,29 +6311,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="38"/>
-      <c r="I40" s="39"/>
-      <c r="J40" s="39"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6358,6 +6333,23 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
25.08.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/August/Others/Cash.xlsx
+++ b/August/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 24.08.19</t>
+    <t>Date: 25.08.19</t>
   </si>
 </sst>
 </file>
@@ -473,12 +473,39 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -488,90 +515,63 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -579,12 +579,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -606,6 +600,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2054,7 +2054,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2076,60 +2076,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2138,10 +2138,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2156,10 +2156,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>50</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2175,10 +2175,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>16</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2194,10 +2194,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>151</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2213,10 +2213,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="34">
         <v>58</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2232,8 +2232,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2249,8 +2249,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2263,10 +2263,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2313,58 +2313,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2374,11 +2374,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2453,60 +2453,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2515,10 +2515,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="41"/>
+      <c r="F31" s="30"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2533,10 +2533,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="34">
         <v>50</v>
       </c>
-      <c r="F32" s="36"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2552,10 +2552,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>116</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2571,10 +2571,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>151</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2590,10 +2590,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="34">
         <v>58</v>
       </c>
-      <c r="F35" s="36"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2609,8 +2609,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2626,8 +2626,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2640,10 +2640,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="32" t="s">
+      <c r="D38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="33"/>
+      <c r="E38" s="42"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2690,58 +2690,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2751,11 +2751,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2783,6 +2783,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2795,32 +2821,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2851,63 +2851,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2917,10 +2917,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="48"/>
+      <c r="F5" s="53"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2935,13 +2935,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="44">
-        <v>78</v>
-      </c>
-      <c r="F6" s="44"/>
+      <c r="E6" s="54">
+        <v>62</v>
+      </c>
+      <c r="F6" s="54"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>78000</v>
+        <v>62000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2954,13 +2954,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="44">
-        <v>114</v>
-      </c>
-      <c r="F7" s="44"/>
+      <c r="E7" s="54">
+        <v>116</v>
+      </c>
+      <c r="F7" s="54"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>57000</v>
+        <v>58000</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2973,13 +2973,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="44">
-        <v>290</v>
-      </c>
-      <c r="F8" s="44"/>
+      <c r="E8" s="54">
+        <v>100</v>
+      </c>
+      <c r="F8" s="54"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>29000</v>
+        <v>10000</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2992,8 +2992,8 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="54"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3009,8 +3009,8 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3026,8 +3026,8 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3040,14 +3040,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="51"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>164000</v>
+        <v>130000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3090,58 +3090,58 @@
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="49"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="49" t="s">
+      <c r="H16" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="46"/>
+      <c r="B17" s="46"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="49"/>
-      <c r="B19" s="49"/>
+      <c r="A19" s="46"/>
+      <c r="B19" s="46"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="50" t="s">
+      <c r="H19" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="26"/>
@@ -3151,9 +3151,9 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="26"/>
@@ -3240,60 +3240,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="51"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="52"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="47" t="s">
+      <c r="A31" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="47"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3302,10 +3302,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="48" t="s">
+      <c r="E32" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="48"/>
+      <c r="F32" s="53"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3320,13 +3320,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="44">
-        <v>78</v>
-      </c>
-      <c r="F33" s="44"/>
+      <c r="E33" s="54">
+        <v>62</v>
+      </c>
+      <c r="F33" s="54"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>78000</v>
+        <v>62000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3339,13 +3339,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="44">
-        <v>114</v>
-      </c>
-      <c r="F34" s="44"/>
+      <c r="E34" s="54">
+        <v>116</v>
+      </c>
+      <c r="F34" s="54"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>57000</v>
+        <v>58000</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3358,13 +3358,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="44">
-        <v>290</v>
-      </c>
-      <c r="F35" s="44"/>
+      <c r="E35" s="54">
+        <v>100</v>
+      </c>
+      <c r="F35" s="54"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>29000</v>
+        <v>10000</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3377,8 +3377,8 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="44"/>
-      <c r="F36" s="44"/>
+      <c r="E36" s="54"/>
+      <c r="F36" s="54"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3394,8 +3394,8 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="54"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -3411,8 +3411,8 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="44"/>
-      <c r="F38" s="44"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="54"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3425,14 +3425,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="54" t="s">
+      <c r="D39" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="55"/>
+      <c r="E39" s="49"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>164000</v>
+        <v>130000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3475,58 +3475,58 @@
       <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="49" t="s">
+      <c r="A43" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="49"/>
+      <c r="B43" s="46"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="49" t="s">
+      <c r="H43" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="49"/>
-      <c r="J43" s="49"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="46"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="53"/>
-      <c r="B44" s="53"/>
+      <c r="A44" s="45"/>
+      <c r="B44" s="45"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="53"/>
-      <c r="I44" s="53"/>
-      <c r="J44" s="53"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
+      <c r="J44" s="45"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="53"/>
-      <c r="B45" s="53"/>
+      <c r="A45" s="45"/>
+      <c r="B45" s="45"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="53"/>
-      <c r="I45" s="53"/>
-      <c r="J45" s="53"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="45"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
-      <c r="A46" s="49"/>
-      <c r="B46" s="49"/>
+      <c r="A46" s="46"/>
+      <c r="B46" s="46"/>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="50" t="s">
+      <c r="H46" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="50"/>
-      <c r="J46" s="50"/>
+      <c r="I46" s="47"/>
+      <c r="J46" s="47"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3536,9 +3536,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3566,6 +3566,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3582,28 +3604,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3634,63 +3634,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3700,10 +3700,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3718,10 +3718,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>68</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3737,10 +3737,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>135</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3756,10 +3756,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>53</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3775,10 +3775,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="34">
         <v>2</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3794,10 +3794,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="36">
+      <c r="E10" s="34">
         <v>5</v>
       </c>
-      <c r="F10" s="36"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3813,8 +3813,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3827,10 +3827,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3877,76 +3877,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="35"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="57"/>
+      <c r="B20" s="56"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4021,60 +4021,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4083,10 +4083,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="56" t="s">
+      <c r="E31" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="56"/>
+      <c r="F31" s="60"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4101,10 +4101,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="60">
+      <c r="E32" s="59">
         <v>68</v>
       </c>
-      <c r="F32" s="60"/>
+      <c r="F32" s="59"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4120,10 +4120,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="60">
+      <c r="E33" s="59">
         <v>135</v>
       </c>
-      <c r="F33" s="60"/>
+      <c r="F33" s="59"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4139,10 +4139,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="60">
+      <c r="E34" s="59">
         <v>53</v>
       </c>
-      <c r="F34" s="60"/>
+      <c r="F34" s="59"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4158,10 +4158,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="60">
+      <c r="E35" s="59">
         <v>2</v>
       </c>
-      <c r="F35" s="60"/>
+      <c r="F35" s="59"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4177,10 +4177,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="60">
+      <c r="E36" s="59">
         <v>5</v>
       </c>
-      <c r="F36" s="60"/>
+      <c r="F36" s="59"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4196,8 +4196,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4210,10 +4210,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="59" t="s">
+      <c r="D38" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="59"/>
+      <c r="E38" s="58"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4260,76 +4260,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="35"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58" t="s">
+      <c r="A46" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="58"/>
+      <c r="B46" s="57"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4357,6 +4357,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4373,30 +4397,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4428,63 +4428,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4494,10 +4494,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4512,10 +4512,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>44</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4531,10 +4531,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>118</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4550,10 +4550,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>510</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4569,8 +4569,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4586,8 +4586,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4603,8 +4603,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4617,10 +4617,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4667,72 +4667,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="61"/>
-      <c r="B20" s="61"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="62"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4807,60 +4807,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4869,10 +4869,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="41"/>
+      <c r="F31" s="30"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4887,10 +4887,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="34">
         <v>44</v>
       </c>
-      <c r="F32" s="36"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4906,10 +4906,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>118</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4925,10 +4925,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>510</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4944,8 +4944,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4961,8 +4961,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4978,8 +4978,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4992,10 +4992,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="62" t="s">
+      <c r="D38" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="62"/>
+      <c r="E38" s="61"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5042,72 +5042,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58"/>
-      <c r="B46" s="58"/>
+      <c r="A46" s="57"/>
+      <c r="B46" s="57"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5135,16 +5135,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5157,24 +5165,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5199,64 +5199,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5267,8 +5267,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5279,8 +5279,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5291,8 +5291,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5303,8 +5303,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5315,8 +5315,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5327,8 +5327,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5338,8 +5338,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5383,52 +5383,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42"/>
-      <c r="B16" s="42"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5438,9 +5438,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5527,60 +5527,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5591,10 +5591,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="56" t="s">
+      <c r="E32" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="56"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5609,10 +5609,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>30</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5628,10 +5628,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>35</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5647,10 +5647,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="34">
         <v>425</v>
       </c>
-      <c r="F35" s="36"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5666,8 +5666,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5683,8 +5683,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5700,10 +5700,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="60">
+      <c r="E38" s="59">
         <v>100</v>
       </c>
-      <c r="F38" s="60"/>
+      <c r="F38" s="59"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5766,58 +5766,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="34"/>
+      <c r="B43" s="43"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="34" t="s">
+      <c r="H43" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="35"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="36"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="35"/>
-      <c r="B46" s="35"/>
+      <c r="A46" s="36"/>
+      <c r="B46" s="36"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
+      <c r="I46" s="43"/>
+      <c r="J46" s="43"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5827,12 +5827,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5845,32 +5871,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5896,177 +5896,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="74">
+      <c r="A5" s="73">
         <v>1</v>
       </c>
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="65">
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="72">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="74"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="65"/>
+      <c r="A6" s="73"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="72"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="74">
+      <c r="A7" s="73">
         <v>2</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="65">
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="72">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="74"/>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="65"/>
+      <c r="A8" s="73"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="72"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="74">
+      <c r="A9" s="73">
         <v>3</v>
       </c>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="65">
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="72">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="74"/>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="65"/>
+      <c r="A10" s="73"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="72"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="74">
+      <c r="A11" s="73">
         <v>4</v>
       </c>
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="65">
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="72">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="74"/>
-      <c r="B12" s="71"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="65"/>
+      <c r="A12" s="73"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="72"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="66" t="s">
+      <c r="A13" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="65">
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="72">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="66"/>
-      <c r="B14" s="66"/>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="65"/>
+      <c r="A14" s="74"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="72"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="40"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6077,10 +6077,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="56" t="s">
+      <c r="E25" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="56"/>
+      <c r="F25" s="60"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6095,8 +6095,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6112,10 +6112,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="36">
+      <c r="E27" s="34">
         <v>30</v>
       </c>
-      <c r="F27" s="36"/>
+      <c r="F27" s="34"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6131,8 +6131,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6148,10 +6148,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="36">
+      <c r="E29" s="34">
         <v>5</v>
       </c>
-      <c r="F29" s="36"/>
+      <c r="F29" s="34"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6167,8 +6167,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="59"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6184,10 +6184,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="60">
+      <c r="E31" s="59">
         <v>2</v>
       </c>
-      <c r="F31" s="60"/>
+      <c r="F31" s="59"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6250,58 +6250,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="34"/>
+      <c r="B36" s="43"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="34" t="s">
+      <c r="H36" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="35"/>
-      <c r="B37" s="35"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="36"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="35"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="36"/>
+      <c r="J37" s="36"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="35"/>
-      <c r="B38" s="35"/>
+      <c r="A38" s="36"/>
+      <c r="B38" s="36"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="35"/>
-      <c r="J38" s="35"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="36"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="35"/>
-      <c r="B39" s="35"/>
+      <c r="A39" s="36"/>
+      <c r="B39" s="36"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="35" t="s">
+      <c r="H39" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
+      <c r="I39" s="43"/>
+      <c r="J39" s="43"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6311,12 +6311,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="31"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6333,23 +6350,6 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
26.08.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/August/Others/Cash.xlsx
+++ b/August/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 25.08.19</t>
+    <t>Date: 26.08.19</t>
   </si>
 </sst>
 </file>
@@ -473,47 +473,71 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -521,34 +545,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -563,15 +566,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -579,6 +579,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -600,12 +606,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2054,7 +2054,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2076,60 +2076,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2138,10 +2138,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2156,10 +2156,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>50</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2175,10 +2175,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>16</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2194,10 +2194,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>151</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2213,10 +2213,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="36">
         <v>58</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2232,8 +2232,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2249,8 +2249,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2263,10 +2263,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2313,58 +2313,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2374,11 +2374,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2453,60 +2453,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2515,10 +2515,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="30"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2533,10 +2533,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="36">
         <v>50</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="36"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2552,10 +2552,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>116</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2571,10 +2571,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>151</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2590,10 +2590,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="36">
         <v>58</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2609,8 +2609,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2626,8 +2626,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2640,10 +2640,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="41" t="s">
+      <c r="D38" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="42"/>
+      <c r="E38" s="33"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2690,58 +2690,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2751,11 +2751,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2783,14 +2783,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2803,24 +2813,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2832,7 +2832,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
       <selection activeCell="H46" sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
@@ -2851,63 +2851,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2917,10 +2917,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="53"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2935,13 +2935,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="54">
-        <v>62</v>
-      </c>
-      <c r="F6" s="54"/>
+      <c r="E6" s="44">
+        <v>48</v>
+      </c>
+      <c r="F6" s="44"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>62000</v>
+        <v>48000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2954,13 +2954,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="54">
-        <v>116</v>
-      </c>
-      <c r="F7" s="54"/>
+      <c r="E7" s="44">
+        <v>66</v>
+      </c>
+      <c r="F7" s="44"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>58000</v>
+        <v>33000</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2973,13 +2973,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="54">
-        <v>100</v>
-      </c>
-      <c r="F8" s="54"/>
+      <c r="E8" s="44">
+        <v>163</v>
+      </c>
+      <c r="F8" s="44"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>10000</v>
+        <v>16300</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2992,11 +2992,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
+      <c r="E9" s="44">
+        <v>14</v>
+      </c>
+      <c r="F9" s="44"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3009,8 +3011,8 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3026,8 +3028,8 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3040,14 +3042,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="55"/>
+      <c r="E12" s="51"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>130000</v>
+        <v>98000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3090,58 +3092,58 @@
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="46"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="46" t="s">
+      <c r="H16" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="46"/>
-      <c r="B17" s="46"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="46"/>
-      <c r="B18" s="46"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="46"/>
-      <c r="B19" s="46"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="47" t="s">
+      <c r="H19" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="26"/>
@@ -3151,9 +3153,9 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="26"/>
@@ -3240,60 +3242,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="50"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="50"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="51"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="52" t="s">
+      <c r="A30" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="52"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="52"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="52" t="s">
+      <c r="A31" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="52"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="52"/>
-      <c r="I31" s="52"/>
-      <c r="J31" s="52"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3302,10 +3304,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="53" t="s">
+      <c r="E32" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="53"/>
+      <c r="F32" s="48"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3320,13 +3322,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="54">
-        <v>62</v>
-      </c>
-      <c r="F33" s="54"/>
+      <c r="E33" s="44">
+        <v>48</v>
+      </c>
+      <c r="F33" s="44"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>62000</v>
+        <v>48000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3339,13 +3341,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="54">
-        <v>116</v>
-      </c>
-      <c r="F34" s="54"/>
+      <c r="E34" s="44">
+        <v>66</v>
+      </c>
+      <c r="F34" s="44"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>58000</v>
+        <v>33000</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3358,13 +3360,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="54">
-        <v>100</v>
-      </c>
-      <c r="F35" s="54"/>
+      <c r="E35" s="44">
+        <v>163</v>
+      </c>
+      <c r="F35" s="44"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>10000</v>
+        <v>16300</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3377,11 +3379,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="54"/>
-      <c r="F36" s="54"/>
+      <c r="E36" s="44">
+        <v>14</v>
+      </c>
+      <c r="F36" s="44"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>700</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3394,8 +3398,8 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
+      <c r="E37" s="44"/>
+      <c r="F37" s="44"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -3411,8 +3415,8 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="54"/>
-      <c r="F38" s="54"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="44"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3425,14 +3429,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="48" t="s">
+      <c r="D39" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="49"/>
+      <c r="E39" s="55"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>130000</v>
+        <v>98000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3475,58 +3479,58 @@
       <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="46" t="s">
+      <c r="A43" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="46"/>
+      <c r="B43" s="49"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="46" t="s">
+      <c r="H43" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="46"/>
-      <c r="J43" s="46"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="45"/>
-      <c r="B44" s="45"/>
+      <c r="A44" s="53"/>
+      <c r="B44" s="53"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="45"/>
-      <c r="I44" s="45"/>
-      <c r="J44" s="45"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="53"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="45"/>
-      <c r="B45" s="45"/>
+      <c r="A45" s="53"/>
+      <c r="B45" s="53"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="45"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="53"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
-      <c r="A46" s="46"/>
-      <c r="B46" s="46"/>
+      <c r="A46" s="49"/>
+      <c r="B46" s="49"/>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="47" t="s">
+      <c r="H46" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="47"/>
-      <c r="J46" s="47"/>
+      <c r="I46" s="50"/>
+      <c r="J46" s="50"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3536,9 +3540,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3566,28 +3570,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3604,6 +3586,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3634,63 +3638,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3700,10 +3704,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3718,10 +3722,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>68</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3737,10 +3741,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>135</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3756,10 +3760,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>53</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3775,10 +3779,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="36">
         <v>2</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3794,10 +3798,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="36">
         <v>5</v>
       </c>
-      <c r="F10" s="34"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3813,8 +3817,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3827,10 +3831,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3877,76 +3881,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="36"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="56" t="s">
+      <c r="A20" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="56"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4021,60 +4025,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4083,10 +4087,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="60" t="s">
+      <c r="E31" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="60"/>
+      <c r="F31" s="56"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4101,10 +4105,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="59">
+      <c r="E32" s="60">
         <v>68</v>
       </c>
-      <c r="F32" s="59"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4120,10 +4124,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="59">
+      <c r="E33" s="60">
         <v>135</v>
       </c>
-      <c r="F33" s="59"/>
+      <c r="F33" s="60"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4139,10 +4143,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="59">
+      <c r="E34" s="60">
         <v>53</v>
       </c>
-      <c r="F34" s="59"/>
+      <c r="F34" s="60"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4158,10 +4162,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="59">
+      <c r="E35" s="60">
         <v>2</v>
       </c>
-      <c r="F35" s="59"/>
+      <c r="F35" s="60"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4177,10 +4181,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="59">
+      <c r="E36" s="60">
         <v>5</v>
       </c>
-      <c r="F36" s="59"/>
+      <c r="F36" s="60"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4196,8 +4200,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4210,10 +4214,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="58" t="s">
+      <c r="D38" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="58"/>
+      <c r="E38" s="59"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4260,76 +4264,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="36" t="s">
+      <c r="A45" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="36"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="57" t="s">
+      <c r="A46" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="57"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4357,30 +4361,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4397,6 +4377,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4428,63 +4432,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4494,10 +4498,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4512,10 +4516,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>44</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4531,10 +4535,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>118</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4550,10 +4554,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>510</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4569,8 +4573,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4586,8 +4590,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4603,8 +4607,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4617,10 +4621,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4667,72 +4671,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="62"/>
-      <c r="B20" s="62"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="61"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4807,60 +4811,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4869,10 +4873,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="30"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4887,10 +4891,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="36">
         <v>44</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="36"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4906,10 +4910,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>118</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4925,10 +4929,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>510</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4944,8 +4948,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4961,8 +4965,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4978,8 +4982,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4992,10 +4996,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="61" t="s">
+      <c r="D38" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="61"/>
+      <c r="E38" s="62"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5042,72 +5046,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="57"/>
-      <c r="B46" s="57"/>
+      <c r="A46" s="58"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5135,6 +5139,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5147,34 +5179,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5199,64 +5203,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5267,8 +5271,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5279,8 +5283,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5291,8 +5295,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5303,8 +5307,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5315,8 +5319,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5327,8 +5331,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5338,8 +5342,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5383,52 +5387,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5438,9 +5442,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5527,60 +5531,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5591,10 +5595,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="60" t="s">
+      <c r="E32" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="60"/>
+      <c r="F32" s="56"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5609,10 +5613,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>30</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5628,10 +5632,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>35</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5647,10 +5651,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="36">
         <v>425</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5666,8 +5670,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5683,8 +5687,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5700,10 +5704,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="59">
+      <c r="E38" s="60">
         <v>100</v>
       </c>
-      <c r="F38" s="59"/>
+      <c r="F38" s="60"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5766,58 +5770,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="43"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="43" t="s">
+      <c r="H43" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="36"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="36"/>
-      <c r="B46" s="36"/>
+      <c r="A46" s="35"/>
+      <c r="B46" s="35"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="36" t="s">
+      <c r="H46" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="43"/>
-      <c r="J46" s="43"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5827,20 +5831,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -5853,24 +5867,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5896,177 +5900,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="73">
+      <c r="A5" s="74">
         <v>1</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="72">
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="65">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="73"/>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="72"/>
+      <c r="A6" s="74"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="65"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="73">
+      <c r="A7" s="74">
         <v>2</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="72">
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="65">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="73"/>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="72"/>
+      <c r="A8" s="74"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="65"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="73">
+      <c r="A9" s="74">
         <v>3</v>
       </c>
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="72">
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="65">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="73"/>
-      <c r="B10" s="65"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="72"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="65"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="73">
+      <c r="A11" s="74">
         <v>4</v>
       </c>
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="72">
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="65">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="73"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="72"/>
+      <c r="A12" s="74"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="65"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="72">
+      <c r="B13" s="66"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="65">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="74"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="72"/>
+      <c r="A14" s="66"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="65"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="40"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="33"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6077,10 +6081,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="60" t="s">
+      <c r="E25" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="60"/>
+      <c r="F25" s="56"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6095,8 +6099,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6112,10 +6116,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="34">
+      <c r="E27" s="36">
         <v>30</v>
       </c>
-      <c r="F27" s="34"/>
+      <c r="F27" s="36"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6131,8 +6135,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6148,10 +6152,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="34">
+      <c r="E29" s="36">
         <v>5</v>
       </c>
-      <c r="F29" s="34"/>
+      <c r="F29" s="36"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6167,8 +6171,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6184,10 +6188,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="59">
+      <c r="E31" s="60">
         <v>2</v>
       </c>
-      <c r="F31" s="59"/>
+      <c r="F31" s="60"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6250,58 +6254,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="43" t="s">
+      <c r="A36" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="43"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="43" t="s">
+      <c r="H36" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="36"/>
-      <c r="B37" s="36"/>
+      <c r="A37" s="35"/>
+      <c r="B37" s="35"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="36"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="36"/>
-      <c r="B38" s="36"/>
+      <c r="A38" s="35"/>
+      <c r="B38" s="35"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="36"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="35"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="36"/>
-      <c r="B39" s="36"/>
+      <c r="A39" s="35"/>
+      <c r="B39" s="35"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="36" t="s">
+      <c r="H39" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="43"/>
-      <c r="J39" s="43"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6311,29 +6315,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="38"/>
-      <c r="I40" s="39"/>
-      <c r="J40" s="39"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6350,6 +6337,23 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
27.08.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/August/Others/Cash.xlsx
+++ b/August/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 26.08.19</t>
+    <t>Date: 27.08.19</t>
   </si>
 </sst>
 </file>
@@ -473,12 +473,39 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -488,90 +515,63 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -579,12 +579,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -606,6 +600,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2054,7 +2054,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2076,60 +2076,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2138,10 +2138,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2156,10 +2156,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>50</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2175,10 +2175,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>16</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2194,10 +2194,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>151</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2213,10 +2213,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="34">
         <v>58</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2232,8 +2232,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2249,8 +2249,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2263,10 +2263,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2313,58 +2313,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2374,11 +2374,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2453,60 +2453,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2515,10 +2515,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="41"/>
+      <c r="F31" s="30"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2533,10 +2533,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="34">
         <v>50</v>
       </c>
-      <c r="F32" s="36"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2552,10 +2552,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>116</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2571,10 +2571,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>151</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2590,10 +2590,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="34">
         <v>58</v>
       </c>
-      <c r="F35" s="36"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2609,8 +2609,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2626,8 +2626,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2640,10 +2640,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="32" t="s">
+      <c r="D38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="33"/>
+      <c r="E38" s="42"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2690,58 +2690,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2751,11 +2751,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2783,6 +2783,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2795,32 +2821,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2832,7 +2832,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H46" sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
@@ -2851,63 +2851,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2917,10 +2917,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="48"/>
+      <c r="F5" s="53"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2935,13 +2935,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="44">
-        <v>48</v>
-      </c>
-      <c r="F6" s="44"/>
+      <c r="E6" s="54">
+        <v>50</v>
+      </c>
+      <c r="F6" s="54"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>48000</v>
+        <v>50000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2954,13 +2954,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="44">
-        <v>66</v>
-      </c>
-      <c r="F7" s="44"/>
+      <c r="E7" s="54">
+        <v>159</v>
+      </c>
+      <c r="F7" s="54"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>33000</v>
+        <v>79500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2973,13 +2973,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="44">
-        <v>163</v>
-      </c>
-      <c r="F8" s="44"/>
+      <c r="E8" s="54">
+        <v>588</v>
+      </c>
+      <c r="F8" s="54"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>16300</v>
+        <v>58800</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2992,10 +2992,10 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="44">
+      <c r="E9" s="54">
         <v>14</v>
       </c>
-      <c r="F9" s="44"/>
+      <c r="F9" s="54"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
         <v>700</v>
@@ -3011,8 +3011,8 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3028,8 +3028,8 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3042,14 +3042,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="51"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>98000</v>
+        <v>189000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3092,58 +3092,58 @@
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="49"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="49" t="s">
+      <c r="H16" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="46"/>
+      <c r="B17" s="46"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="49"/>
-      <c r="B19" s="49"/>
+      <c r="A19" s="46"/>
+      <c r="B19" s="46"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="50" t="s">
+      <c r="H19" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="26"/>
@@ -3153,9 +3153,9 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="26"/>
@@ -3242,60 +3242,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="51"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="52"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="47" t="s">
+      <c r="A31" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="47"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3304,10 +3304,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="48" t="s">
+      <c r="E32" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="48"/>
+      <c r="F32" s="53"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3322,13 +3322,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="44">
-        <v>48</v>
-      </c>
-      <c r="F33" s="44"/>
+      <c r="E33" s="54">
+        <v>50</v>
+      </c>
+      <c r="F33" s="54"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>48000</v>
+        <v>50000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3341,13 +3341,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="44">
-        <v>66</v>
-      </c>
-      <c r="F34" s="44"/>
+      <c r="E34" s="54">
+        <v>159</v>
+      </c>
+      <c r="F34" s="54"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>33000</v>
+        <v>79500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3360,13 +3360,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="44">
-        <v>163</v>
-      </c>
-      <c r="F35" s="44"/>
+      <c r="E35" s="54">
+        <v>588</v>
+      </c>
+      <c r="F35" s="54"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>16300</v>
+        <v>58800</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3379,10 +3379,10 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="44">
+      <c r="E36" s="54">
         <v>14</v>
       </c>
-      <c r="F36" s="44"/>
+      <c r="F36" s="54"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
         <v>700</v>
@@ -3398,8 +3398,8 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="54"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -3415,8 +3415,8 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="44"/>
-      <c r="F38" s="44"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="54"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3429,14 +3429,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="54" t="s">
+      <c r="D39" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="55"/>
+      <c r="E39" s="49"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>98000</v>
+        <v>189000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3479,58 +3479,58 @@
       <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="49" t="s">
+      <c r="A43" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="49"/>
+      <c r="B43" s="46"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="49" t="s">
+      <c r="H43" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="49"/>
-      <c r="J43" s="49"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="46"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="53"/>
-      <c r="B44" s="53"/>
+      <c r="A44" s="45"/>
+      <c r="B44" s="45"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="53"/>
-      <c r="I44" s="53"/>
-      <c r="J44" s="53"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
+      <c r="J44" s="45"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="53"/>
-      <c r="B45" s="53"/>
+      <c r="A45" s="45"/>
+      <c r="B45" s="45"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="53"/>
-      <c r="I45" s="53"/>
-      <c r="J45" s="53"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="45"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
-      <c r="A46" s="49"/>
-      <c r="B46" s="49"/>
+      <c r="A46" s="46"/>
+      <c r="B46" s="46"/>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="50" t="s">
+      <c r="H46" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="50"/>
-      <c r="J46" s="50"/>
+      <c r="I46" s="47"/>
+      <c r="J46" s="47"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3540,9 +3540,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3570,6 +3570,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3586,28 +3608,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3638,63 +3638,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3704,10 +3704,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3722,10 +3722,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>68</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3741,10 +3741,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>135</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3760,10 +3760,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>53</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3779,10 +3779,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="34">
         <v>2</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3798,10 +3798,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="36">
+      <c r="E10" s="34">
         <v>5</v>
       </c>
-      <c r="F10" s="36"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3817,8 +3817,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3831,10 +3831,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3881,76 +3881,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="35"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="57"/>
+      <c r="B20" s="56"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4025,60 +4025,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4087,10 +4087,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="56" t="s">
+      <c r="E31" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="56"/>
+      <c r="F31" s="60"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4105,10 +4105,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="60">
+      <c r="E32" s="59">
         <v>68</v>
       </c>
-      <c r="F32" s="60"/>
+      <c r="F32" s="59"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4124,10 +4124,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="60">
+      <c r="E33" s="59">
         <v>135</v>
       </c>
-      <c r="F33" s="60"/>
+      <c r="F33" s="59"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4143,10 +4143,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="60">
+      <c r="E34" s="59">
         <v>53</v>
       </c>
-      <c r="F34" s="60"/>
+      <c r="F34" s="59"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4162,10 +4162,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="60">
+      <c r="E35" s="59">
         <v>2</v>
       </c>
-      <c r="F35" s="60"/>
+      <c r="F35" s="59"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4181,10 +4181,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="60">
+      <c r="E36" s="59">
         <v>5</v>
       </c>
-      <c r="F36" s="60"/>
+      <c r="F36" s="59"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4200,8 +4200,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4214,10 +4214,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="59" t="s">
+      <c r="D38" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="59"/>
+      <c r="E38" s="58"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4264,76 +4264,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="35"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58" t="s">
+      <c r="A46" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="58"/>
+      <c r="B46" s="57"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4361,6 +4361,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4377,30 +4401,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4432,63 +4432,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4498,10 +4498,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4516,10 +4516,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>44</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4535,10 +4535,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>118</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4554,10 +4554,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>510</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4573,8 +4573,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4590,8 +4590,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4607,8 +4607,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4621,10 +4621,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4671,72 +4671,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="61"/>
-      <c r="B20" s="61"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="62"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4811,60 +4811,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4873,10 +4873,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="41"/>
+      <c r="F31" s="30"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4891,10 +4891,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="34">
         <v>44</v>
       </c>
-      <c r="F32" s="36"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4910,10 +4910,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>118</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4929,10 +4929,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>510</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4948,8 +4948,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4965,8 +4965,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4982,8 +4982,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4996,10 +4996,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="62" t="s">
+      <c r="D38" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="62"/>
+      <c r="E38" s="61"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5046,72 +5046,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58"/>
-      <c r="B46" s="58"/>
+      <c r="A46" s="57"/>
+      <c r="B46" s="57"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5139,16 +5139,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5161,24 +5169,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5203,64 +5203,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5271,8 +5271,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5283,8 +5283,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5295,8 +5295,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5307,8 +5307,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5319,8 +5319,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5331,8 +5331,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5342,8 +5342,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5387,52 +5387,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42"/>
-      <c r="B16" s="42"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5442,9 +5442,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5531,60 +5531,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5595,10 +5595,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="56" t="s">
+      <c r="E32" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="56"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5613,10 +5613,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>30</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5632,10 +5632,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>35</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5651,10 +5651,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="34">
         <v>425</v>
       </c>
-      <c r="F35" s="36"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5670,8 +5670,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5687,8 +5687,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5704,10 +5704,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="60">
+      <c r="E38" s="59">
         <v>100</v>
       </c>
-      <c r="F38" s="60"/>
+      <c r="F38" s="59"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5770,58 +5770,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="34"/>
+      <c r="B43" s="43"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="34" t="s">
+      <c r="H43" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="35"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="36"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="35"/>
-      <c r="B46" s="35"/>
+      <c r="A46" s="36"/>
+      <c r="B46" s="36"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
+      <c r="I46" s="43"/>
+      <c r="J46" s="43"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5831,12 +5831,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5849,32 +5875,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5900,177 +5900,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="74">
+      <c r="A5" s="73">
         <v>1</v>
       </c>
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="65">
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="72">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="74"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="65"/>
+      <c r="A6" s="73"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="72"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="74">
+      <c r="A7" s="73">
         <v>2</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="65">
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="72">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="74"/>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="65"/>
+      <c r="A8" s="73"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="72"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="74">
+      <c r="A9" s="73">
         <v>3</v>
       </c>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="65">
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="72">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="74"/>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="65"/>
+      <c r="A10" s="73"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="72"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="74">
+      <c r="A11" s="73">
         <v>4</v>
       </c>
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="65">
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="72">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="74"/>
-      <c r="B12" s="71"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="65"/>
+      <c r="A12" s="73"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="72"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="66" t="s">
+      <c r="A13" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="65">
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="72">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="66"/>
-      <c r="B14" s="66"/>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="65"/>
+      <c r="A14" s="74"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="72"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="40"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6081,10 +6081,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="56" t="s">
+      <c r="E25" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="56"/>
+      <c r="F25" s="60"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6099,8 +6099,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6116,10 +6116,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="36">
+      <c r="E27" s="34">
         <v>30</v>
       </c>
-      <c r="F27" s="36"/>
+      <c r="F27" s="34"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6135,8 +6135,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6152,10 +6152,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="36">
+      <c r="E29" s="34">
         <v>5</v>
       </c>
-      <c r="F29" s="36"/>
+      <c r="F29" s="34"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6171,8 +6171,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="59"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6188,10 +6188,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="60">
+      <c r="E31" s="59">
         <v>2</v>
       </c>
-      <c r="F31" s="60"/>
+      <c r="F31" s="59"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6254,58 +6254,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="34"/>
+      <c r="B36" s="43"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="34" t="s">
+      <c r="H36" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="35"/>
-      <c r="B37" s="35"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="36"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="35"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="36"/>
+      <c r="J37" s="36"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="35"/>
-      <c r="B38" s="35"/>
+      <c r="A38" s="36"/>
+      <c r="B38" s="36"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="35"/>
-      <c r="J38" s="35"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="36"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="35"/>
-      <c r="B39" s="35"/>
+      <c r="A39" s="36"/>
+      <c r="B39" s="36"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="35" t="s">
+      <c r="H39" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
+      <c r="I39" s="43"/>
+      <c r="J39" s="43"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6315,12 +6315,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="31"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6337,23 +6354,6 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
28.08.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/August/Others/Cash.xlsx
+++ b/August/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 27.08.19</t>
+    <t>Date: 28.08.19</t>
   </si>
 </sst>
 </file>
@@ -473,47 +473,71 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -521,34 +545,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -563,15 +566,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -579,6 +579,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -600,12 +606,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2054,7 +2054,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2076,60 +2076,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2138,10 +2138,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2156,10 +2156,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>50</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2175,10 +2175,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>16</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2194,10 +2194,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>151</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2213,10 +2213,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="36">
         <v>58</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2232,8 +2232,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2249,8 +2249,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2263,10 +2263,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2313,58 +2313,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2374,11 +2374,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2453,60 +2453,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2515,10 +2515,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="30"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2533,10 +2533,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="36">
         <v>50</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="36"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2552,10 +2552,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>116</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2571,10 +2571,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>151</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2590,10 +2590,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="36">
         <v>58</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2609,8 +2609,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2626,8 +2626,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2640,10 +2640,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="41" t="s">
+      <c r="D38" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="42"/>
+      <c r="E38" s="33"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2690,58 +2690,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2751,11 +2751,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2783,14 +2783,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2803,24 +2813,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2851,63 +2851,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="50"/>
-      <c r="G1" s="50"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="51"/>
-      <c r="J3" s="51"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
-      <c r="D4" s="52"/>
-      <c r="E4" s="52"/>
-      <c r="F4" s="52"/>
-      <c r="G4" s="52"/>
-      <c r="H4" s="52"/>
-      <c r="I4" s="52"/>
-      <c r="J4" s="52"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="47"/>
+      <c r="I4" s="47"/>
+      <c r="J4" s="47"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2917,10 +2917,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="53"/>
+      <c r="F5" s="48"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2935,13 +2935,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="54">
-        <v>50</v>
-      </c>
-      <c r="F6" s="54"/>
+      <c r="E6" s="44">
+        <v>42</v>
+      </c>
+      <c r="F6" s="44"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>50000</v>
+        <v>42000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2954,13 +2954,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="54">
-        <v>159</v>
-      </c>
-      <c r="F7" s="54"/>
+      <c r="E7" s="44">
+        <v>100</v>
+      </c>
+      <c r="F7" s="44"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>79500</v>
+        <v>50000</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2973,13 +2973,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="54">
-        <v>588</v>
-      </c>
-      <c r="F8" s="54"/>
+      <c r="E8" s="44">
+        <v>319</v>
+      </c>
+      <c r="F8" s="44"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>58800</v>
+        <v>31900</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2992,13 +2992,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="54">
-        <v>14</v>
-      </c>
-      <c r="F9" s="54"/>
+      <c r="E9" s="44">
+        <v>25</v>
+      </c>
+      <c r="F9" s="44"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>700</v>
+        <v>1250</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3011,11 +3011,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
+      <c r="E10" s="44">
+        <v>73</v>
+      </c>
+      <c r="F10" s="44"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1460</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3028,11 +3030,13 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
+      <c r="E11" s="44">
+        <v>39</v>
+      </c>
+      <c r="F11" s="44"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>390</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3042,14 +3046,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="55"/>
+      <c r="E12" s="51"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>189000</v>
+        <v>127000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3092,58 +3096,58 @@
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="46"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="46" t="s">
+      <c r="H16" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="46"/>
-      <c r="J16" s="46"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="46"/>
-      <c r="B17" s="46"/>
+      <c r="A17" s="49"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="46"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="46"/>
-      <c r="B18" s="46"/>
+      <c r="A18" s="49"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="46"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="46"/>
-      <c r="B19" s="46"/>
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="47" t="s">
+      <c r="H19" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="50"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="26"/>
@@ -3153,9 +3157,9 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="26"/>
@@ -3242,60 +3246,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="50" t="s">
+      <c r="A28" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="50"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="50"/>
+      <c r="B28" s="45"/>
+      <c r="C28" s="45"/>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45"/>
+      <c r="F28" s="45"/>
+      <c r="G28" s="45"/>
+      <c r="H28" s="45"/>
+      <c r="I28" s="45"/>
+      <c r="J28" s="45"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="51"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
-      <c r="G29" s="51"/>
-      <c r="H29" s="51"/>
-      <c r="I29" s="51"/>
-      <c r="J29" s="51"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
+      <c r="J29" s="46"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="52" t="s">
+      <c r="A30" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="52"/>
-      <c r="C30" s="52"/>
-      <c r="D30" s="52"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="52"/>
-      <c r="G30" s="52"/>
-      <c r="H30" s="52"/>
-      <c r="I30" s="52"/>
-      <c r="J30" s="52"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="47"/>
+      <c r="G30" s="47"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="47"/>
+      <c r="J30" s="47"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="52" t="s">
+      <c r="A31" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="52"/>
-      <c r="C31" s="52"/>
-      <c r="D31" s="52"/>
-      <c r="E31" s="52"/>
-      <c r="F31" s="52"/>
-      <c r="G31" s="52"/>
-      <c r="H31" s="52"/>
-      <c r="I31" s="52"/>
-      <c r="J31" s="52"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3304,10 +3308,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="53" t="s">
+      <c r="E32" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="53"/>
+      <c r="F32" s="48"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3322,13 +3326,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="54">
-        <v>50</v>
-      </c>
-      <c r="F33" s="54"/>
+      <c r="E33" s="44">
+        <v>42</v>
+      </c>
+      <c r="F33" s="44"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>50000</v>
+        <v>42000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3341,13 +3345,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="54">
-        <v>159</v>
-      </c>
-      <c r="F34" s="54"/>
+      <c r="E34" s="44">
+        <v>100</v>
+      </c>
+      <c r="F34" s="44"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>79500</v>
+        <v>50000</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3360,13 +3364,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="54">
-        <v>588</v>
-      </c>
-      <c r="F35" s="54"/>
+      <c r="E35" s="44">
+        <v>319</v>
+      </c>
+      <c r="F35" s="44"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>58800</v>
+        <v>31900</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3379,13 +3383,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="54">
-        <v>14</v>
-      </c>
-      <c r="F36" s="54"/>
+      <c r="E36" s="44">
+        <v>25</v>
+      </c>
+      <c r="F36" s="44"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>700</v>
+        <v>1250</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3398,11 +3402,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="54"/>
-      <c r="F37" s="54"/>
+      <c r="E37" s="44">
+        <v>73</v>
+      </c>
+      <c r="F37" s="44"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>0</v>
+        <v>1460</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3415,11 +3421,13 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="54"/>
-      <c r="F38" s="54"/>
+      <c r="E38" s="44">
+        <v>39</v>
+      </c>
+      <c r="F38" s="44"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>390</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3429,14 +3437,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="48" t="s">
+      <c r="D39" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="49"/>
+      <c r="E39" s="55"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>189000</v>
+        <v>127000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3479,58 +3487,58 @@
       <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="46" t="s">
+      <c r="A43" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="46"/>
+      <c r="B43" s="49"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="46" t="s">
+      <c r="H43" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="46"/>
-      <c r="J43" s="46"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="45"/>
-      <c r="B44" s="45"/>
+      <c r="A44" s="53"/>
+      <c r="B44" s="53"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="45"/>
-      <c r="I44" s="45"/>
-      <c r="J44" s="45"/>
+      <c r="H44" s="53"/>
+      <c r="I44" s="53"/>
+      <c r="J44" s="53"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="45"/>
-      <c r="B45" s="45"/>
+      <c r="A45" s="53"/>
+      <c r="B45" s="53"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="45"/>
+      <c r="H45" s="53"/>
+      <c r="I45" s="53"/>
+      <c r="J45" s="53"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
-      <c r="A46" s="46"/>
-      <c r="B46" s="46"/>
+      <c r="A46" s="49"/>
+      <c r="B46" s="49"/>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="47" t="s">
+      <c r="H46" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="47"/>
-      <c r="J46" s="47"/>
+      <c r="I46" s="50"/>
+      <c r="J46" s="50"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3540,9 +3548,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3570,28 +3578,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3608,6 +3594,28 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3638,63 +3646,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3704,10 +3712,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3722,10 +3730,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>68</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3741,10 +3749,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>135</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3760,10 +3768,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>53</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3779,10 +3787,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34">
+      <c r="E9" s="36">
         <v>2</v>
       </c>
-      <c r="F9" s="34"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3798,10 +3806,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34">
+      <c r="E10" s="36">
         <v>5</v>
       </c>
-      <c r="F10" s="34"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3817,8 +3825,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3831,10 +3839,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3881,76 +3889,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="36"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="56" t="s">
+      <c r="A20" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="56"/>
+      <c r="B20" s="57"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4025,60 +4033,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4087,10 +4095,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="60" t="s">
+      <c r="E31" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="60"/>
+      <c r="F31" s="56"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4105,10 +4113,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="59">
+      <c r="E32" s="60">
         <v>68</v>
       </c>
-      <c r="F32" s="59"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4124,10 +4132,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="59">
+      <c r="E33" s="60">
         <v>135</v>
       </c>
-      <c r="F33" s="59"/>
+      <c r="F33" s="60"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4143,10 +4151,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="59">
+      <c r="E34" s="60">
         <v>53</v>
       </c>
-      <c r="F34" s="59"/>
+      <c r="F34" s="60"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4162,10 +4170,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="59">
+      <c r="E35" s="60">
         <v>2</v>
       </c>
-      <c r="F35" s="59"/>
+      <c r="F35" s="60"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4181,10 +4189,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="59">
+      <c r="E36" s="60">
         <v>5</v>
       </c>
-      <c r="F36" s="59"/>
+      <c r="F36" s="60"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4200,8 +4208,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4214,10 +4222,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="58" t="s">
+      <c r="D38" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="58"/>
+      <c r="E38" s="59"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4264,76 +4272,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="36" t="s">
+      <c r="A45" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="36"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="57" t="s">
+      <c r="A46" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="57"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4361,30 +4369,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4401,6 +4385,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4432,63 +4440,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="32" t="s">
+      <c r="A3" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4498,10 +4506,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="30"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4516,10 +4524,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="34">
+      <c r="E6" s="36">
         <v>44</v>
       </c>
-      <c r="F6" s="34"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4535,10 +4543,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="34">
+      <c r="E7" s="36">
         <v>118</v>
       </c>
-      <c r="F7" s="34"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4554,10 +4562,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="36">
         <v>510</v>
       </c>
-      <c r="F8" s="34"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4573,8 +4581,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4590,8 +4598,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4607,8 +4615,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4621,10 +4629,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="30"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4671,72 +4679,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35" t="s">
+      <c r="H16" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37" t="s">
+      <c r="H19" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="62"/>
-      <c r="B20" s="62"/>
+      <c r="A20" s="61"/>
+      <c r="B20" s="61"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38" t="s">
+      <c r="H20" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4811,60 +4819,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="31"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="32" t="s">
+      <c r="A28" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
+      <c r="B28" s="38"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="38"/>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
+      <c r="J29" s="39"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="33"/>
-      <c r="H30" s="33"/>
-      <c r="I30" s="33"/>
-      <c r="J30" s="33"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4873,10 +4881,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="30"/>
+      <c r="F31" s="41"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4891,10 +4899,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="34">
+      <c r="E32" s="36">
         <v>44</v>
       </c>
-      <c r="F32" s="34"/>
+      <c r="F32" s="36"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4910,10 +4918,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>118</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4929,10 +4937,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>510</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4948,8 +4956,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4965,8 +4973,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4982,8 +4990,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="36"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4996,10 +5004,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="61" t="s">
+      <c r="D38" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="61"/>
+      <c r="E38" s="62"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5046,72 +5054,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="43"/>
+      <c r="B42" s="34"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="43" t="s">
+      <c r="H42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="43"/>
-      <c r="J42" s="43"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="36"/>
-      <c r="B43" s="36"/>
+      <c r="A43" s="35"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="36"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36" t="s">
+      <c r="H45" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="57"/>
-      <c r="B46" s="57"/>
+      <c r="A46" s="58"/>
+      <c r="B46" s="58"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="38" t="s">
+      <c r="H46" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5139,6 +5147,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5151,34 +5187,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5203,64 +5211,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
+      <c r="A4" s="40"/>
+      <c r="B4" s="40"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5271,8 +5279,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5283,8 +5291,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5295,8 +5303,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5307,8 +5315,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5319,8 +5327,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5331,8 +5339,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5342,8 +5350,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5387,52 +5395,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="42"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="42"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="35"/>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
+      <c r="H17" s="42"/>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="42"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="36"/>
-      <c r="B19" s="36"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5442,9 +5450,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5531,60 +5539,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
-      <c r="I29" s="32"/>
-      <c r="J29" s="32"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="39"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="I30" s="39"/>
+      <c r="J30" s="39"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="33"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="33"/>
+      <c r="B31" s="40"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="40"/>
+      <c r="E31" s="40"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="40"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5595,10 +5603,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="60" t="s">
+      <c r="E32" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="60"/>
+      <c r="F32" s="56"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5613,10 +5621,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="34">
+      <c r="E33" s="36">
         <v>30</v>
       </c>
-      <c r="F33" s="34"/>
+      <c r="F33" s="36"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5632,10 +5640,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="34">
+      <c r="E34" s="36">
         <v>35</v>
       </c>
-      <c r="F34" s="34"/>
+      <c r="F34" s="36"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5651,10 +5659,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="34">
+      <c r="E35" s="36">
         <v>425</v>
       </c>
-      <c r="F35" s="34"/>
+      <c r="F35" s="36"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5670,8 +5678,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5687,8 +5695,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
+      <c r="E37" s="60"/>
+      <c r="F37" s="60"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5704,10 +5712,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="59">
+      <c r="E38" s="60">
         <v>100</v>
       </c>
-      <c r="F38" s="59"/>
+      <c r="F38" s="60"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5770,58 +5778,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="43" t="s">
+      <c r="A43" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="43"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="43" t="s">
+      <c r="H43" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="43"/>
-      <c r="J43" s="43"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="36"/>
-      <c r="B44" s="36"/>
+      <c r="A44" s="35"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="36"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="36"/>
-      <c r="B45" s="36"/>
+      <c r="A45" s="35"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="36"/>
-      <c r="I45" s="36"/>
-      <c r="J45" s="36"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="36"/>
-      <c r="B46" s="36"/>
+      <c r="A46" s="35"/>
+      <c r="B46" s="35"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="36" t="s">
+      <c r="H46" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="43"/>
-      <c r="J46" s="43"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5831,20 +5839,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="31"/>
+      <c r="J47" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -5857,24 +5875,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5900,177 +5908,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="73">
+      <c r="A5" s="74">
         <v>1</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="65"/>
-      <c r="G5" s="72">
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="65">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="73"/>
-      <c r="B6" s="65"/>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="72"/>
+      <c r="A6" s="74"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="65"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="73">
+      <c r="A7" s="74">
         <v>2</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="65"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="65"/>
-      <c r="G7" s="72">
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="65">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="73"/>
-      <c r="B8" s="65"/>
-      <c r="C8" s="65"/>
-      <c r="D8" s="65"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="65"/>
-      <c r="G8" s="72"/>
+      <c r="A8" s="74"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="67"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="67"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="65"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="73">
+      <c r="A9" s="74">
         <v>3</v>
       </c>
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="65"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="72">
+      <c r="C9" s="67"/>
+      <c r="D9" s="67"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="65">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="73"/>
-      <c r="B10" s="65"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="72"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="67"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="65"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="73">
+      <c r="A11" s="74">
         <v>4</v>
       </c>
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="68"/>
-      <c r="G11" s="72">
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="70"/>
+      <c r="G11" s="65">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="73"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="70"/>
-      <c r="D12" s="70"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="72"/>
+      <c r="A12" s="74"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="65"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="72">
+      <c r="B13" s="66"/>
+      <c r="C13" s="66"/>
+      <c r="D13" s="66"/>
+      <c r="E13" s="66"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="65">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="74"/>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="72"/>
+      <c r="A14" s="66"/>
+      <c r="B14" s="66"/>
+      <c r="C14" s="66"/>
+      <c r="D14" s="66"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="66"/>
+      <c r="G14" s="65"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="40"/>
+      <c r="B23" s="39"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="39"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="33"/>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
-      <c r="J24" s="33"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="40"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6081,10 +6089,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="60" t="s">
+      <c r="E25" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="60"/>
+      <c r="F25" s="56"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6099,8 +6107,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6116,10 +6124,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="34">
+      <c r="E27" s="36">
         <v>30</v>
       </c>
-      <c r="F27" s="34"/>
+      <c r="F27" s="36"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6135,8 +6143,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6152,10 +6160,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="34">
+      <c r="E29" s="36">
         <v>5</v>
       </c>
-      <c r="F29" s="34"/>
+      <c r="F29" s="36"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6171,8 +6179,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="59"/>
-      <c r="F30" s="59"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="60"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6188,10 +6196,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="59">
+      <c r="E31" s="60">
         <v>2</v>
       </c>
-      <c r="F31" s="59"/>
+      <c r="F31" s="60"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6254,58 +6262,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="43" t="s">
+      <c r="A36" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="43"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="43" t="s">
+      <c r="H36" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="36"/>
-      <c r="B37" s="36"/>
+      <c r="A37" s="35"/>
+      <c r="B37" s="35"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="36"/>
+      <c r="H37" s="35"/>
+      <c r="I37" s="35"/>
+      <c r="J37" s="35"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="36"/>
-      <c r="B38" s="36"/>
+      <c r="A38" s="35"/>
+      <c r="B38" s="35"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="36"/>
+      <c r="H38" s="35"/>
+      <c r="I38" s="35"/>
+      <c r="J38" s="35"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="36"/>
-      <c r="B39" s="36"/>
+      <c r="A39" s="35"/>
+      <c r="B39" s="35"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="36" t="s">
+      <c r="H39" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="43"/>
-      <c r="J39" s="43"/>
+      <c r="I39" s="34"/>
+      <c r="J39" s="34"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6315,29 +6323,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="38"/>
-      <c r="I40" s="39"/>
-      <c r="J40" s="39"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="31"/>
+      <c r="J40" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6354,6 +6345,23 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
01.09.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/August/Others/Cash.xlsx
+++ b/August/Others/Cash.xlsx
@@ -101,7 +101,7 @@
     <t>Total=</t>
   </si>
   <si>
-    <t>Date: 29.08.19</t>
+    <t>Date: 31.08.19</t>
   </si>
 </sst>
 </file>
@@ -473,12 +473,39 @@
     <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -488,90 +515,63 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -579,12 +579,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -606,6 +600,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2054,7 +2054,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2076,60 +2076,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2138,10 +2138,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2156,10 +2156,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>50</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2175,10 +2175,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>16</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2194,10 +2194,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>151</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2213,10 +2213,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="34">
         <v>58</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2232,8 +2232,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2249,8 +2249,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2263,10 +2263,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2313,58 +2313,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2374,11 +2374,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2453,60 +2453,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2515,10 +2515,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="41"/>
+      <c r="F31" s="30"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2533,10 +2533,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="34">
         <v>50</v>
       </c>
-      <c r="F32" s="36"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2552,10 +2552,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>116</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2571,10 +2571,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>151</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2590,10 +2590,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="34">
         <v>58</v>
       </c>
-      <c r="F35" s="36"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2609,8 +2609,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2626,8 +2626,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2640,10 +2640,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="32" t="s">
+      <c r="D38" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="33"/>
+      <c r="E38" s="42"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2690,58 +2690,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2751,11 +2751,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2783,6 +2783,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2795,32 +2821,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2832,8 +2832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H46" sqref="A1:J46"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="O56" sqref="O56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2851,63 +2851,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2917,10 +2917,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="48"/>
+      <c r="F5" s="53"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2935,13 +2935,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="44">
-        <v>47</v>
-      </c>
-      <c r="F6" s="44"/>
+      <c r="E6" s="54">
+        <v>3</v>
+      </c>
+      <c r="F6" s="54"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>47000</v>
+        <v>3000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2954,13 +2954,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="44">
-        <v>127</v>
-      </c>
-      <c r="F7" s="44"/>
+      <c r="E7" s="54">
+        <v>200</v>
+      </c>
+      <c r="F7" s="54"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>63500</v>
+        <v>100000</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2973,13 +2973,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="44">
-        <v>150</v>
-      </c>
-      <c r="F8" s="44"/>
+      <c r="E8" s="54">
+        <v>302</v>
+      </c>
+      <c r="F8" s="54"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>15000</v>
+        <v>30200</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -2992,13 +2992,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="44">
-        <v>108</v>
-      </c>
-      <c r="F9" s="44"/>
+      <c r="E9" s="54">
+        <v>16</v>
+      </c>
+      <c r="F9" s="54"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>5400</v>
+        <v>800</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3011,13 +3011,11 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="44">
-        <v>105</v>
-      </c>
-      <c r="F10" s="44"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="54"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>2100</v>
+        <v>0</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3030,8 +3028,8 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3044,14 +3042,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="51"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>133000</v>
+        <v>134000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3094,58 +3092,58 @@
       <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="49" t="s">
+      <c r="A16" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="49"/>
+      <c r="B16" s="46"/>
       <c r="C16" s="28"/>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
       <c r="F16" s="28"/>
       <c r="G16" s="28"/>
-      <c r="H16" s="49" t="s">
+      <c r="H16" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="46"/>
+      <c r="B17" s="46"/>
       <c r="C17" s="28"/>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
       <c r="F17" s="28"/>
       <c r="G17" s="28"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="46"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="46"/>
+      <c r="B18" s="46"/>
       <c r="C18" s="28"/>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
       <c r="F18" s="28"/>
       <c r="G18" s="28"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
-      <c r="A19" s="49"/>
-      <c r="B19" s="49"/>
+      <c r="A19" s="46"/>
+      <c r="B19" s="46"/>
       <c r="C19" s="28"/>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-      <c r="H19" s="50" t="s">
+      <c r="H19" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="50"/>
-      <c r="J19" s="50"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="26"/>
@@ -3155,9 +3153,9 @@
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="53"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="45"/>
+      <c r="J20" s="45"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="26"/>
@@ -3244,60 +3242,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="45" t="s">
+      <c r="A28" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="45"/>
-      <c r="C28" s="45"/>
-      <c r="D28" s="45"/>
-      <c r="E28" s="45"/>
-      <c r="F28" s="45"/>
-      <c r="G28" s="45"/>
-      <c r="H28" s="45"/>
-      <c r="I28" s="45"/>
-      <c r="J28" s="45"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="50"/>
+      <c r="H28" s="50"/>
+      <c r="I28" s="50"/>
+      <c r="J28" s="50"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="46" t="s">
+      <c r="A29" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
+      <c r="B29" s="51"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="51"/>
+      <c r="G29" s="51"/>
+      <c r="H29" s="51"/>
+      <c r="I29" s="51"/>
+      <c r="J29" s="51"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="47"/>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="47"/>
-      <c r="H30" s="47"/>
-      <c r="I30" s="47"/>
-      <c r="J30" s="47"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="52"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="47" t="s">
+      <c r="A31" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="B31" s="47"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="47"/>
-      <c r="J31" s="47"/>
+      <c r="B31" s="52"/>
+      <c r="C31" s="52"/>
+      <c r="D31" s="52"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3306,10 +3304,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="48" t="s">
+      <c r="E32" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="48"/>
+      <c r="F32" s="53"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3324,13 +3322,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="44">
-        <v>47</v>
-      </c>
-      <c r="F33" s="44"/>
+      <c r="E33" s="54">
+        <v>3</v>
+      </c>
+      <c r="F33" s="54"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>47000</v>
+        <v>3000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3343,13 +3341,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="44">
-        <v>127</v>
-      </c>
-      <c r="F34" s="44"/>
+      <c r="E34" s="54">
+        <v>200</v>
+      </c>
+      <c r="F34" s="54"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>63500</v>
+        <v>100000</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3362,13 +3360,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="44">
-        <v>150</v>
-      </c>
-      <c r="F35" s="44"/>
+      <c r="E35" s="54">
+        <v>302</v>
+      </c>
+      <c r="F35" s="54"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>15000</v>
+        <v>30200</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3381,13 +3379,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="44">
-        <v>108</v>
-      </c>
-      <c r="F36" s="44"/>
+      <c r="E36" s="54">
+        <v>16</v>
+      </c>
+      <c r="F36" s="54"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>5400</v>
+        <v>800</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3400,13 +3398,11 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="44">
-        <v>105</v>
-      </c>
-      <c r="F37" s="44"/>
+      <c r="E37" s="54"/>
+      <c r="F37" s="54"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>2100</v>
+        <v>0</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3419,8 +3415,8 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="44"/>
-      <c r="F38" s="44"/>
+      <c r="E38" s="54"/>
+      <c r="F38" s="54"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -3433,14 +3429,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="54" t="s">
+      <c r="D39" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="55"/>
+      <c r="E39" s="49"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>133000</v>
+        <v>134000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3483,58 +3479,58 @@
       <c r="J42" s="26"/>
     </row>
     <row r="43" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A43" s="49" t="s">
+      <c r="A43" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="49"/>
+      <c r="B43" s="46"/>
       <c r="C43" s="28"/>
       <c r="D43" s="28"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="49" t="s">
+      <c r="H43" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="49"/>
-      <c r="J43" s="49"/>
+      <c r="I43" s="46"/>
+      <c r="J43" s="46"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="53"/>
-      <c r="B44" s="53"/>
+      <c r="A44" s="45"/>
+      <c r="B44" s="45"/>
       <c r="C44" s="26"/>
       <c r="D44" s="26"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="53"/>
-      <c r="I44" s="53"/>
-      <c r="J44" s="53"/>
+      <c r="H44" s="45"/>
+      <c r="I44" s="45"/>
+      <c r="J44" s="45"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="53"/>
-      <c r="B45" s="53"/>
+      <c r="A45" s="45"/>
+      <c r="B45" s="45"/>
       <c r="C45" s="26"/>
       <c r="D45" s="26"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="53"/>
-      <c r="I45" s="53"/>
-      <c r="J45" s="53"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="45"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
-      <c r="A46" s="49"/>
-      <c r="B46" s="49"/>
+      <c r="A46" s="46"/>
+      <c r="B46" s="46"/>
       <c r="C46" s="28"/>
       <c r="D46" s="28"/>
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="50" t="s">
+      <c r="H46" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="50"/>
-      <c r="J46" s="50"/>
+      <c r="I46" s="47"/>
+      <c r="J46" s="47"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3544,9 +3540,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3574,6 +3570,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="D12:E12"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A43:B43"/>
@@ -3590,28 +3608,6 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3642,63 +3638,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3708,10 +3704,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3726,10 +3722,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>68</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3745,10 +3741,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>135</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3764,10 +3760,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>53</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3783,10 +3779,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="34">
         <v>2</v>
       </c>
-      <c r="F9" s="36"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3802,10 +3798,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="36">
+      <c r="E10" s="34">
         <v>5</v>
       </c>
-      <c r="F10" s="36"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3821,8 +3817,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3835,10 +3831,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3885,76 +3881,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="35"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="57"/>
+      <c r="B20" s="56"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4029,60 +4025,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4091,10 +4087,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="56" t="s">
+      <c r="E31" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="56"/>
+      <c r="F31" s="60"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4109,10 +4105,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="60">
+      <c r="E32" s="59">
         <v>68</v>
       </c>
-      <c r="F32" s="60"/>
+      <c r="F32" s="59"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4128,10 +4124,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="60">
+      <c r="E33" s="59">
         <v>135</v>
       </c>
-      <c r="F33" s="60"/>
+      <c r="F33" s="59"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4147,10 +4143,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="60">
+      <c r="E34" s="59">
         <v>53</v>
       </c>
-      <c r="F34" s="60"/>
+      <c r="F34" s="59"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4166,10 +4162,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="60">
+      <c r="E35" s="59">
         <v>2</v>
       </c>
-      <c r="F35" s="60"/>
+      <c r="F35" s="59"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4185,10 +4181,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="60">
+      <c r="E36" s="59">
         <v>5</v>
       </c>
-      <c r="F36" s="60"/>
+      <c r="F36" s="59"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4204,8 +4200,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4218,10 +4214,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="59" t="s">
+      <c r="D38" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="59"/>
+      <c r="E38" s="58"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4268,76 +4264,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="35"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58" t="s">
+      <c r="A46" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="58"/>
+      <c r="B46" s="57"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4365,6 +4361,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4381,30 +4401,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4436,63 +4432,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="40" t="s">
+      <c r="A4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4502,10 +4498,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4520,10 +4516,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="34">
         <v>44</v>
       </c>
-      <c r="F6" s="36"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4539,10 +4535,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="34">
         <v>118</v>
       </c>
-      <c r="F7" s="36"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4558,10 +4554,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="34">
         <v>510</v>
       </c>
-      <c r="F8" s="36"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4577,8 +4573,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4594,8 +4590,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4611,8 +4607,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4625,10 +4621,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="41"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4675,72 +4671,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="42" t="s">
+      <c r="A16" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="42"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43" t="s">
+      <c r="H19" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="61"/>
-      <c r="B20" s="61"/>
+      <c r="A20" s="62"/>
+      <c r="B20" s="62"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30" t="s">
+      <c r="H20" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4815,60 +4811,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="37"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
-      <c r="F28" s="38"/>
-      <c r="G28" s="38"/>
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
-      <c r="J28" s="38"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="39" t="s">
+      <c r="A29" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="40" t="s">
+      <c r="A30" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="40"/>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4877,10 +4873,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="41" t="s">
+      <c r="E31" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="41"/>
+      <c r="F31" s="30"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4895,10 +4891,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="36">
+      <c r="E32" s="34">
         <v>44</v>
       </c>
-      <c r="F32" s="36"/>
+      <c r="F32" s="34"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4914,10 +4910,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>118</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4933,10 +4929,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>510</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4952,8 +4948,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4969,8 +4965,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4986,8 +4982,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5000,10 +4996,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="62" t="s">
+      <c r="D38" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="62"/>
+      <c r="E38" s="61"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5050,72 +5046,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="34" t="s">
+      <c r="A42" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="34"/>
+      <c r="B42" s="43"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="34" t="s">
+      <c r="H42" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="34"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="35"/>
-      <c r="B43" s="35"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="36"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="35"/>
-      <c r="I43" s="35"/>
-      <c r="J43" s="35"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="36"/>
+      <c r="J43" s="36"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="34"/>
-      <c r="J45" s="34"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="58"/>
-      <c r="B46" s="58"/>
+      <c r="A46" s="57"/>
+      <c r="B46" s="57"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="30" t="s">
+      <c r="H46" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5143,16 +5139,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5165,24 +5169,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5207,64 +5203,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="38"/>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="38"/>
-      <c r="J3" s="38"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="40"/>
-      <c r="J4" s="40"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5275,8 +5271,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5287,8 +5283,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5299,8 +5295,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="34"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5311,8 +5307,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5323,8 +5319,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5335,8 +5331,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5346,8 +5342,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5391,52 +5387,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="42"/>
-      <c r="B16" s="42"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="42"/>
-      <c r="B17" s="42"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="42"/>
-      <c r="B18" s="42"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5446,9 +5442,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5535,60 +5531,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="31"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
-      <c r="J29" s="38"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="40"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="40" t="s">
+      <c r="A31" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="33"/>
+      <c r="H31" s="33"/>
+      <c r="I31" s="33"/>
+      <c r="J31" s="33"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5599,10 +5595,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="56" t="s">
+      <c r="E32" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="56"/>
+      <c r="F32" s="60"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5617,10 +5613,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="36">
+      <c r="E33" s="34">
         <v>30</v>
       </c>
-      <c r="F33" s="36"/>
+      <c r="F33" s="34"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5636,10 +5632,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="36">
+      <c r="E34" s="34">
         <v>35</v>
       </c>
-      <c r="F34" s="36"/>
+      <c r="F34" s="34"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5655,10 +5651,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="36">
+      <c r="E35" s="34">
         <v>425</v>
       </c>
-      <c r="F35" s="36"/>
+      <c r="F35" s="34"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5674,8 +5670,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5691,8 +5687,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="60"/>
-      <c r="F37" s="60"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5708,10 +5704,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="60">
+      <c r="E38" s="59">
         <v>100</v>
       </c>
-      <c r="F38" s="60"/>
+      <c r="F38" s="59"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5774,58 +5770,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="34" t="s">
+      <c r="A43" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="34"/>
+      <c r="B43" s="43"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="34" t="s">
+      <c r="H43" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="34"/>
-      <c r="J43" s="34"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="35"/>
-      <c r="B44" s="35"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="36"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="36"/>
+      <c r="J44" s="36"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="35"/>
-      <c r="B45" s="35"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="35"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="35"/>
+      <c r="H45" s="36"/>
+      <c r="I45" s="36"/>
+      <c r="J45" s="36"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="35"/>
-      <c r="B46" s="35"/>
+      <c r="A46" s="36"/>
+      <c r="B46" s="36"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
+      <c r="I46" s="43"/>
+      <c r="J46" s="43"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5835,12 +5831,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
+      <c r="H47" s="38"/>
+      <c r="I47" s="39"/>
+      <c r="J47" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5853,32 +5875,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5904,177 +5900,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="74">
+      <c r="A5" s="73">
         <v>1</v>
       </c>
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="65">
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="72">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="74"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="67"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="65"/>
+      <c r="A6" s="73"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="72"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="74">
+      <c r="A7" s="73">
         <v>2</v>
       </c>
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="65">
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="72">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="74"/>
-      <c r="B8" s="67"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="67"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="65"/>
+      <c r="A8" s="73"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="72"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="74">
+      <c r="A9" s="73">
         <v>3</v>
       </c>
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="65" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="67"/>
-      <c r="D9" s="67"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="67"/>
-      <c r="G9" s="65">
+      <c r="C9" s="65"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="65"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="72">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="74"/>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="65"/>
+      <c r="A10" s="73"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="72"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="74">
+      <c r="A11" s="73">
         <v>4</v>
       </c>
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="65">
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="72">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="74"/>
-      <c r="B12" s="71"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="72"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="65"/>
+      <c r="A12" s="73"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="70"/>
+      <c r="D12" s="70"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="72"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="66" t="s">
+      <c r="A13" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66"/>
-      <c r="E13" s="66"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="65">
+      <c r="B13" s="74"/>
+      <c r="C13" s="74"/>
+      <c r="D13" s="74"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="74"/>
+      <c r="G13" s="72">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="66"/>
-      <c r="B14" s="66"/>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66"/>
-      <c r="E14" s="66"/>
-      <c r="F14" s="66"/>
-      <c r="G14" s="65"/>
+      <c r="A14" s="74"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="74"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="74"/>
+      <c r="G14" s="72"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
+      <c r="B23" s="40"/>
+      <c r="C23" s="40"/>
+      <c r="D23" s="40"/>
+      <c r="E23" s="40"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="40"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="40"/>
-      <c r="B24" s="40"/>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="40"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
+      <c r="A24" s="33"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="33"/>
+      <c r="I24" s="33"/>
+      <c r="J24" s="33"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6085,10 +6081,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="56" t="s">
+      <c r="E25" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="56"/>
+      <c r="F25" s="60"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6103,8 +6099,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6120,10 +6116,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="36">
+      <c r="E27" s="34">
         <v>30</v>
       </c>
-      <c r="F27" s="36"/>
+      <c r="F27" s="34"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6139,8 +6135,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6156,10 +6152,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="36">
+      <c r="E29" s="34">
         <v>5</v>
       </c>
-      <c r="F29" s="36"/>
+      <c r="F29" s="34"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6175,8 +6171,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
+      <c r="E30" s="59"/>
+      <c r="F30" s="59"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6192,10 +6188,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="60">
+      <c r="E31" s="59">
         <v>2</v>
       </c>
-      <c r="F31" s="60"/>
+      <c r="F31" s="59"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6258,58 +6254,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="34"/>
+      <c r="B36" s="43"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="34" t="s">
+      <c r="H36" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="35"/>
-      <c r="B37" s="35"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="36"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="35"/>
-      <c r="I37" s="35"/>
-      <c r="J37" s="35"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="36"/>
+      <c r="J37" s="36"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="35"/>
-      <c r="B38" s="35"/>
+      <c r="A38" s="36"/>
+      <c r="B38" s="36"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="35"/>
-      <c r="I38" s="35"/>
-      <c r="J38" s="35"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="36"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="35"/>
-      <c r="B39" s="35"/>
+      <c r="A39" s="36"/>
+      <c r="B39" s="36"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="35" t="s">
+      <c r="H39" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
+      <c r="I39" s="43"/>
+      <c r="J39" s="43"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6319,12 +6315,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="31"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="39"/>
+      <c r="J40" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6341,23 +6354,6 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>